<commit_message>
20200915 CRE20-003-01	Enhancement on Programme or Scheme using batch upload – Phase 1 20200915 CRE20-007-01	Launch of 2020_21 VSS, RVP and School Outreach Vaccination – Phase 1
</commit_message>
<xml_diff>
--- a/EHS2019/EHS/ExcelGenerator/Template/eHSVF001-VaccinationFileTemplate-MMR.xlsx
+++ b/EHS2019/EHS/ExcelGenerator/Template/eHSVF001-VaccinationFileTemplate-MMR.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\EHS2019\EHS\ExcelGenerator\Template\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="195" windowWidth="18195" windowHeight="11505"/>
   </bookViews>
@@ -255,7 +260,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="dd\ mmm\ yyyy"/>
     <numFmt numFmtId="165" formatCode="dd\ mmm\ yyyy\ hh:mm"/>
@@ -1554,6 +1559,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1601,7 +1609,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1636,7 +1644,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1845,14 +1853,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="41.5703125" style="12" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" style="35" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" style="35" customWidth="1"/>
     <col min="3" max="3" width="16.85546875" style="33" customWidth="1"/>
     <col min="4" max="16384" width="9.140625" style="12"/>
   </cols>
@@ -1944,102 +1952,120 @@
       <c r="C18" s="36"/>
     </row>
     <row r="19" spans="1:3" s="25" customFormat="1">
-      <c r="A19" s="25" t="s">
-        <v>53</v>
-      </c>
       <c r="B19" s="36"/>
       <c r="C19" s="36"/>
     </row>
     <row r="20" spans="1:3" s="25" customFormat="1">
-      <c r="A20" s="25" t="s">
-        <v>52</v>
-      </c>
       <c r="B20" s="36"/>
       <c r="C20" s="36"/>
     </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="12" t="s">
+    <row r="21" spans="1:3" s="25" customFormat="1">
+      <c r="A21" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" s="36"/>
+      <c r="C21" s="36"/>
+    </row>
+    <row r="22" spans="1:3" s="25" customFormat="1">
+      <c r="A22" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" s="36"/>
+      <c r="C22" s="36"/>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="37"/>
-    </row>
-    <row r="22" spans="1:3" s="16" customFormat="1">
-      <c r="A22" s="17" t="s">
+      <c r="B23" s="37"/>
+    </row>
+    <row r="24" spans="1:3" s="16" customFormat="1">
+      <c r="A24" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="37"/>
-      <c r="C22" s="33"/>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="B23" s="37"/>
-    </row>
-    <row r="24" spans="1:3" s="17" customFormat="1">
       <c r="B24" s="37"/>
       <c r="C24" s="33"/>
     </row>
-    <row r="25" spans="1:3" s="17" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A25" s="24" t="s">
-        <v>65</v>
+    <row r="25" spans="1:3">
+      <c r="A25" s="17" t="s">
+        <v>63</v>
       </c>
       <c r="B25" s="37"/>
-      <c r="C25" s="33"/>
-    </row>
-    <row r="26" spans="1:3" s="17" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A26" s="24" t="s">
-        <v>64</v>
-      </c>
+    </row>
+    <row r="26" spans="1:3" s="17" customFormat="1">
       <c r="B26" s="37"/>
       <c r="C26" s="33"/>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" s="17" customFormat="1" ht="31.5" customHeight="1">
+      <c r="A27" s="24" t="s">
+        <v>65</v>
+      </c>
       <c r="B27" s="37"/>
-    </row>
-    <row r="28" spans="1:3" s="17" customFormat="1">
-      <c r="A28" s="22" t="s">
+      <c r="C27" s="33"/>
+    </row>
+    <row r="28" spans="1:3" s="17" customFormat="1" ht="31.5" customHeight="1">
+      <c r="A28" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="B28" s="37"/>
+      <c r="C28" s="33"/>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="B29" s="37"/>
+    </row>
+    <row r="30" spans="1:3" s="17" customFormat="1">
+      <c r="A30" s="22" t="s">
         <v>66</v>
-      </c>
-      <c r="B28" s="38"/>
-      <c r="C28" s="33"/>
-    </row>
-    <row r="29" spans="1:3" s="25" customFormat="1">
-      <c r="A29" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="B29" s="38"/>
-      <c r="C29" s="33"/>
-    </row>
-    <row r="30" spans="1:3" s="25" customFormat="1">
-      <c r="A30" s="22" t="s">
-        <v>77</v>
       </c>
       <c r="B30" s="38"/>
       <c r="C30" s="33"/>
     </row>
     <row r="31" spans="1:3" s="25" customFormat="1">
-      <c r="A31" s="22"/>
+      <c r="A31" s="22" t="s">
+        <v>76</v>
+      </c>
       <c r="B31" s="38"/>
       <c r="C31" s="33"/>
     </row>
-    <row r="32" spans="1:3" s="17" customFormat="1">
-      <c r="A32" s="23" t="s">
-        <v>67</v>
+    <row r="32" spans="1:3" s="25" customFormat="1">
+      <c r="A32" s="22" t="s">
+        <v>77</v>
       </c>
       <c r="B32" s="38"/>
       <c r="C32" s="33"/>
     </row>
-    <row r="33" spans="1:3" s="17" customFormat="1">
+    <row r="33" spans="1:3" s="25" customFormat="1">
       <c r="A33" s="22"/>
-      <c r="B33" s="39"/>
+      <c r="B33" s="38"/>
       <c r="C33" s="33"/>
     </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="12" t="s">
+    <row r="34" spans="1:3" s="17" customFormat="1">
+      <c r="A34" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="B34" s="38"/>
+      <c r="C34" s="33"/>
+    </row>
+    <row r="35" spans="1:3" s="25" customFormat="1">
+      <c r="A35" s="23"/>
+      <c r="B35" s="38"/>
+      <c r="C35" s="33"/>
+    </row>
+    <row r="36" spans="1:3" s="25" customFormat="1">
+      <c r="A36" s="23"/>
+      <c r="B36" s="38"/>
+      <c r="C36" s="33"/>
+    </row>
+    <row r="37" spans="1:3" s="17" customFormat="1">
+      <c r="A37" s="22"/>
+      <c r="B37" s="39"/>
+      <c r="C37" s="33"/>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B34" s="40"/>
+      <c r="B38" s="40"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
20201006 INT20-0033	Fix eHSVF001-Template-SIV and sorting in DPAR report 20201007 CRE20-007-03	Launch of 2020_21 VSS, RVP and School Outreach Vaccination – Phase 3 20201007 CRE20-009	To add document requirement for DA Recipients 20201007 CRE20-003-01a	Enhancement on Programme or Scheme using batch upload – Phase 1a 20201007 CRE20-005-02	eHRSS Patient Portal - Phase 2 20201008 INT20-0034	Tune Perfomance on get EHS Vaccine 20201009 INT20-0035	Tune Performance on search account 20201011 INT20-0036 	Fix category name too long in the report D0033 20201011 CRS20-013	To update the HA MingLiu font files in the eHS(S) 20201020 CRE20-003-02	Enhancement on Programme or Scheme using batch upload – Phase 2 20201021 INT20-0038 	Fix display of serach criteria in VU CTM & CTE 20201022 INT20-0039	Fix save in pre-check assign date 20201023 INT20-0040	Grant DELETE permission on DB table - PatientPortalDoctorList_File 20201027 INT20-0041 	Fix click background when please wait icon is shown
</commit_message>
<xml_diff>
--- a/EHS2019/EHS/ExcelGenerator/Template/eHSVF001-VaccinationFileTemplate-MMR.xlsx
+++ b/EHS2019/EHS/ExcelGenerator/Template/eHSVF001-VaccinationFileTemplate-MMR.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\EHS2019\EHS\ExcelGenerator\Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\EHS2019_BatchUpload\ExcelGenerator\bin\Debug\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,15 +13,16 @@
   </bookViews>
   <sheets>
     <sheet name="Batch" sheetId="4" r:id="rId1"/>
-    <sheet name="ReportTemplate" sheetId="1" r:id="rId2"/>
-    <sheet name="Remark" sheetId="2" r:id="rId3"/>
+    <sheet name="Follow Up Client" sheetId="5" r:id="rId2"/>
+    <sheet name="ReportTemplate" sheetId="1" r:id="rId3"/>
+    <sheet name="Remark" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="79">
   <si>
     <t>Temp account no.</t>
   </si>
@@ -255,22 +256,26 @@
   </si>
   <si>
     <t xml:space="preserve"> - 2nd Dose</t>
+  </si>
+  <si>
+    <t>Require follow up</t>
+    <phoneticPr fontId="37" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="dd\ mmm\ yyyy"/>
-    <numFmt numFmtId="165" formatCode="dd\ mmm\ yyyy\ hh:mm"/>
-    <numFmt numFmtId="166" formatCode="yyyy/mm/dd"/>
+    <numFmt numFmtId="176" formatCode="dd\ mmm\ yyyy"/>
+    <numFmt numFmtId="177" formatCode="dd\ mmm\ yyyy\ hh:mm"/>
+    <numFmt numFmtId="178" formatCode="yyyy/mm/dd"/>
   </numFmts>
-  <fonts count="37">
+  <fonts count="38" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -278,28 +283,28 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -307,7 +312,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -355,7 +360,7 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="1"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -363,7 +368,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="1"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -371,7 +376,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -379,7 +384,7 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -516,21 +521,28 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="新細明體"/>
+      <family val="2"/>
+      <charset val="136"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -670,7 +682,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -923,6 +935,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="156">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1206,7 +1229,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1258,7 +1281,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1291,7 +1314,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1303,7 +1326,7 @@
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="5" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1361,6 +1384,12 @@
     </xf>
     <xf numFmtId="49" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1393,6 +1422,12 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="156">
@@ -1553,7 +1588,43 @@
     <cellStyle name="一般_Book3" xfId="2"/>
     <cellStyle name="一般_eHSA0001-eHS HCVS Statistic for FHB (for year 2009)" xfId="3"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="5">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1857,7 +1928,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="41.5703125" style="12" customWidth="1"/>
     <col min="2" max="2" width="22.7109375" style="35" customWidth="1"/>
@@ -1865,209 +1936,210 @@
     <col min="4" max="16384" width="9.140625" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="11" customFormat="1" ht="15.75">
+    <row r="1" spans="1:3" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>12</v>
       </c>
       <c r="B1" s="15"/>
       <c r="C1" s="32"/>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="9"/>
       <c r="B2" s="10"/>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>62</v>
       </c>
       <c r="B3" s="13"/>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>13</v>
       </c>
       <c r="B4" s="14"/>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="14"/>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="9"/>
       <c r="B6" s="14"/>
     </row>
-    <row r="7" spans="1:3" s="17" customFormat="1">
+    <row r="7" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
         <v>22</v>
       </c>
       <c r="B7" s="14"/>
       <c r="C7" s="33"/>
     </row>
-    <row r="8" spans="1:3" s="17" customFormat="1">
+    <row r="8" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9"/>
       <c r="B8" s="14"/>
       <c r="C8" s="33"/>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="9"/>
       <c r="B9" s="14"/>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
         <v>17</v>
       </c>
       <c r="B10" s="34"/>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="16" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="25" customFormat="1">
+    <row r="15" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B15" s="35"/>
       <c r="C15" s="33"/>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C16" s="35"/>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="36"/>
       <c r="C17" s="36"/>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>20</v>
       </c>
       <c r="B18" s="36"/>
       <c r="C18" s="36"/>
     </row>
-    <row r="19" spans="1:3" s="25" customFormat="1">
+    <row r="19" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B19" s="36"/>
       <c r="C19" s="36"/>
     </row>
-    <row r="20" spans="1:3" s="25" customFormat="1">
+    <row r="20" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B20" s="36"/>
       <c r="C20" s="36"/>
     </row>
-    <row r="21" spans="1:3" s="25" customFormat="1">
+    <row r="21" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="25" t="s">
         <v>53</v>
       </c>
       <c r="B21" s="36"/>
       <c r="C21" s="36"/>
     </row>
-    <row r="22" spans="1:3" s="25" customFormat="1">
+    <row r="22" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="25" t="s">
         <v>52</v>
       </c>
       <c r="B22" s="36"/>
       <c r="C22" s="36"/>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="12" t="s">
         <v>23</v>
       </c>
       <c r="B23" s="37"/>
     </row>
-    <row r="24" spans="1:3" s="16" customFormat="1">
+    <row r="24" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="17" t="s">
         <v>21</v>
       </c>
       <c r="B24" s="37"/>
       <c r="C24" s="33"/>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="17" t="s">
         <v>63</v>
       </c>
       <c r="B25" s="37"/>
     </row>
-    <row r="26" spans="1:3" s="17" customFormat="1">
+    <row r="26" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B26" s="37"/>
       <c r="C26" s="33"/>
     </row>
-    <row r="27" spans="1:3" s="17" customFormat="1" ht="31.5" customHeight="1">
+    <row r="27" spans="1:3" s="17" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="24" t="s">
         <v>65</v>
       </c>
       <c r="B27" s="37"/>
       <c r="C27" s="33"/>
     </row>
-    <row r="28" spans="1:3" s="17" customFormat="1" ht="31.5" customHeight="1">
+    <row r="28" spans="1:3" s="17" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="24" t="s">
         <v>64</v>
       </c>
       <c r="B28" s="37"/>
       <c r="C28" s="33"/>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B29" s="37"/>
     </row>
-    <row r="30" spans="1:3" s="17" customFormat="1">
+    <row r="30" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="22" t="s">
         <v>66</v>
       </c>
       <c r="B30" s="38"/>
       <c r="C30" s="33"/>
     </row>
-    <row r="31" spans="1:3" s="25" customFormat="1">
+    <row r="31" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="22" t="s">
         <v>76</v>
       </c>
       <c r="B31" s="38"/>
       <c r="C31" s="33"/>
     </row>
-    <row r="32" spans="1:3" s="25" customFormat="1">
+    <row r="32" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="22" t="s">
         <v>77</v>
       </c>
       <c r="B32" s="38"/>
       <c r="C32" s="33"/>
     </row>
-    <row r="33" spans="1:3" s="25" customFormat="1">
+    <row r="33" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="22"/>
       <c r="B33" s="38"/>
       <c r="C33" s="33"/>
     </row>
-    <row r="34" spans="1:3" s="17" customFormat="1">
+    <row r="34" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="23" t="s">
         <v>67</v>
       </c>
       <c r="B34" s="38"/>
       <c r="C34" s="33"/>
     </row>
-    <row r="35" spans="1:3" s="25" customFormat="1">
+    <row r="35" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="23"/>
       <c r="B35" s="38"/>
       <c r="C35" s="33"/>
     </row>
-    <row r="36" spans="1:3" s="25" customFormat="1">
+    <row r="36" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="23"/>
       <c r="B36" s="38"/>
       <c r="C36" s="33"/>
     </row>
-    <row r="37" spans="1:3" s="17" customFormat="1">
+    <row r="37" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="22"/>
       <c r="B37" s="39"/>
       <c r="C37" s="33"/>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="12" t="s">
         <v>16</v>
       </c>
       <c r="B38" s="40"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="37" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter>
@@ -2080,112 +2152,117 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z197"/>
+  <dimension ref="A1:AA197"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8" customWidth="1"/>
-    <col min="2" max="2" width="6.42578125" customWidth="1"/>
-    <col min="3" max="3" width="5.42578125" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="8" style="28" customWidth="1"/>
+    <col min="2" max="2" width="6.42578125" style="28" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" style="28" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" style="28" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" style="28" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" style="28" customWidth="1"/>
     <col min="7" max="7" width="4.140625" style="28" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.42578125" style="61" customWidth="1"/>
-    <col min="9" max="9" width="8.85546875" customWidth="1"/>
-    <col min="10" max="10" width="4.7109375" customWidth="1"/>
-    <col min="11" max="11" width="14" customWidth="1"/>
-    <col min="12" max="12" width="6.85546875" style="28" customWidth="1"/>
+    <col min="9" max="9" width="8.85546875" style="28" customWidth="1"/>
+    <col min="10" max="10" width="4.7109375" style="28" customWidth="1"/>
+    <col min="11" max="11" width="14" style="28" customWidth="1"/>
+    <col min="12" max="12" width="8.7109375" style="28" customWidth="1"/>
     <col min="13" max="13" width="10.85546875" style="28" customWidth="1"/>
-    <col min="14" max="14" width="14" customWidth="1"/>
-    <col min="15" max="15" width="7.5703125" customWidth="1"/>
-    <col min="16" max="16" width="13.140625" customWidth="1"/>
-    <col min="17" max="17" width="22.42578125" customWidth="1"/>
-    <col min="19" max="19" width="4.7109375" customWidth="1"/>
-    <col min="20" max="20" width="12.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.42578125" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="31.28515625" style="48" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14" style="28" customWidth="1"/>
+    <col min="15" max="15" width="7.5703125" style="28" customWidth="1"/>
+    <col min="16" max="16" width="13.140625" style="28" customWidth="1"/>
+    <col min="17" max="17" width="22.42578125" style="28" customWidth="1"/>
+    <col min="18" max="18" width="10.42578125" style="28" customWidth="1"/>
+    <col min="19" max="19" width="9.140625" style="28"/>
+    <col min="20" max="20" width="4.7109375" style="28" customWidth="1"/>
+    <col min="21" max="21" width="12.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.42578125" style="28" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="8.28515625" style="28" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9" style="28" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="8.85546875" style="28" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="31.28515625" style="48" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="8.5703125" style="28" bestFit="1" customWidth="1"/>
+    <col min="28" max="16384" width="9.140625" style="28"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="4" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A1" s="62" t="s">
+    <row r="1" spans="1:27" s="4" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="64" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
+      <c r="I1" s="64"/>
       <c r="J1" s="3"/>
-      <c r="K1" s="63" t="s">
+      <c r="K1" s="65" t="s">
         <v>54</v>
       </c>
-      <c r="L1" s="63"/>
-      <c r="M1" s="63"/>
-      <c r="N1" s="63"/>
-      <c r="O1" s="63"/>
-      <c r="P1" s="63"/>
-      <c r="Q1" s="64"/>
-      <c r="R1" s="65"/>
-      <c r="S1" s="42"/>
-      <c r="T1" s="66" t="s">
+      <c r="L1" s="65"/>
+      <c r="M1" s="65"/>
+      <c r="N1" s="65"/>
+      <c r="O1" s="65"/>
+      <c r="P1" s="65"/>
+      <c r="Q1" s="66"/>
+      <c r="R1" s="75"/>
+      <c r="S1" s="67"/>
+      <c r="T1" s="42"/>
+      <c r="U1" s="68" t="s">
         <v>11</v>
       </c>
-      <c r="U1" s="63"/>
-      <c r="V1" s="63"/>
-      <c r="W1" s="63"/>
-      <c r="X1" s="63"/>
-      <c r="Y1" s="63"/>
-      <c r="Z1" s="63"/>
-    </row>
-    <row r="2" spans="1:26" s="4" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A2" s="72"/>
-      <c r="B2" s="72"/>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72"/>
-      <c r="H2" s="72"/>
-      <c r="I2" s="72"/>
+      <c r="V1" s="65"/>
+      <c r="W1" s="65"/>
+      <c r="X1" s="65"/>
+      <c r="Y1" s="65"/>
+      <c r="Z1" s="65"/>
+      <c r="AA1" s="65"/>
+    </row>
+    <row r="2" spans="1:27" s="4" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="74"/>
+      <c r="B2" s="74"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
       <c r="J2" s="3"/>
-      <c r="K2" s="67" t="s">
+      <c r="K2" s="69" t="s">
         <v>61</v>
       </c>
-      <c r="L2" s="68"/>
-      <c r="M2" s="69"/>
-      <c r="N2" s="67" t="s">
+      <c r="L2" s="70"/>
+      <c r="M2" s="71"/>
+      <c r="N2" s="69" t="s">
         <v>55</v>
       </c>
-      <c r="O2" s="68"/>
-      <c r="P2" s="68"/>
+      <c r="O2" s="70"/>
+      <c r="P2" s="70"/>
       <c r="Q2" s="51"/>
-      <c r="R2" s="70" t="s">
+      <c r="R2" s="51"/>
+      <c r="S2" s="72" t="s">
         <v>75</v>
       </c>
-      <c r="S2" s="42"/>
-      <c r="T2" s="55"/>
-      <c r="U2" s="56"/>
-      <c r="V2" s="53" t="s">
+      <c r="T2" s="42"/>
+      <c r="U2" s="55"/>
+      <c r="V2" s="56"/>
+      <c r="W2" s="62" t="s">
         <v>74</v>
       </c>
-      <c r="W2" s="58"/>
       <c r="X2" s="58"/>
-      <c r="Y2" s="54"/>
-      <c r="Z2" s="57"/>
-    </row>
-    <row r="3" spans="1:26" s="7" customFormat="1" ht="58.5" customHeight="1">
+      <c r="Y2" s="58"/>
+      <c r="Z2" s="63"/>
+      <c r="AA2" s="57"/>
+    </row>
+    <row r="3" spans="1:27" s="7" customFormat="1" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>69</v>
       </c>
@@ -2235,1520 +2312,1420 @@
       <c r="Q3" s="52" t="s">
         <v>68</v>
       </c>
-      <c r="R3" s="71"/>
-      <c r="S3" s="43"/>
-      <c r="T3" s="41" t="s">
+      <c r="R3" s="76" t="s">
+        <v>78</v>
+      </c>
+      <c r="S3" s="73"/>
+      <c r="T3" s="43"/>
+      <c r="U3" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="U3" s="2" t="s">
+      <c r="V3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="V3" s="2" t="s">
+      <c r="W3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="W3" s="2" t="s">
+      <c r="X3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="X3" s="2" t="s">
+      <c r="Y3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="Y3" s="30" t="s">
+      <c r="Z3" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="Z3" s="2" t="s">
+      <c r="AA3" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:26" s="18" customFormat="1" ht="15.75">
+    <row r="4" spans="1:27" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D4" s="19"/>
       <c r="G4" s="47"/>
       <c r="H4" s="59"/>
       <c r="J4" s="20"/>
-      <c r="L4" s="29"/>
-      <c r="M4" s="29"/>
       <c r="P4" s="21"/>
-      <c r="S4" s="44"/>
-      <c r="T4" s="21"/>
-      <c r="Y4" s="49"/>
-    </row>
-    <row r="5" spans="1:26" s="18" customFormat="1" ht="15.75">
+      <c r="T4" s="44"/>
+      <c r="U4" s="21"/>
+      <c r="Z4" s="49"/>
+    </row>
+    <row r="5" spans="1:27" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D5" s="19"/>
       <c r="G5" s="47"/>
       <c r="H5" s="59"/>
       <c r="J5" s="20"/>
-      <c r="K5" s="29"/>
-      <c r="L5" s="29"/>
-      <c r="M5" s="29"/>
       <c r="P5" s="21"/>
-      <c r="S5" s="45"/>
-      <c r="T5" s="21"/>
-      <c r="Y5" s="49"/>
-    </row>
-    <row r="6" spans="1:26" s="18" customFormat="1" ht="15.75">
+      <c r="T5" s="45"/>
+      <c r="U5" s="21"/>
+      <c r="Z5" s="49"/>
+    </row>
+    <row r="6" spans="1:27" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D6" s="19"/>
       <c r="G6" s="47"/>
       <c r="H6" s="59"/>
-      <c r="I6" s="27"/>
       <c r="J6" s="20"/>
-      <c r="L6" s="29"/>
-      <c r="M6" s="29"/>
       <c r="P6" s="21"/>
-      <c r="S6" s="45"/>
-      <c r="T6" s="21"/>
-      <c r="Y6" s="49"/>
-    </row>
-    <row r="7" spans="1:26" s="18" customFormat="1" ht="15.75">
+      <c r="T6" s="45"/>
+      <c r="U6" s="21"/>
+      <c r="Z6" s="49"/>
+    </row>
+    <row r="7" spans="1:27" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D7" s="19"/>
       <c r="G7" s="47"/>
       <c r="H7" s="59"/>
       <c r="J7" s="20"/>
-      <c r="L7" s="29"/>
-      <c r="M7" s="29"/>
       <c r="P7" s="21"/>
-      <c r="S7" s="45"/>
-      <c r="T7" s="21"/>
-      <c r="Y7" s="49"/>
-    </row>
-    <row r="8" spans="1:26" s="18" customFormat="1" ht="15.75">
+      <c r="T7" s="45"/>
+      <c r="U7" s="21"/>
+      <c r="Z7" s="49"/>
+    </row>
+    <row r="8" spans="1:27" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D8" s="19"/>
       <c r="G8" s="47"/>
       <c r="H8" s="59"/>
       <c r="J8" s="20"/>
-      <c r="L8" s="29"/>
-      <c r="M8" s="29"/>
       <c r="P8" s="21"/>
-      <c r="S8" s="45"/>
-      <c r="T8" s="21"/>
-      <c r="Y8" s="49"/>
-    </row>
-    <row r="9" spans="1:26" s="18" customFormat="1" ht="15.75">
+      <c r="T8" s="45"/>
+      <c r="U8" s="21"/>
+      <c r="Z8" s="49"/>
+    </row>
+    <row r="9" spans="1:27" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D9" s="19"/>
       <c r="G9" s="47"/>
       <c r="H9" s="59"/>
       <c r="J9" s="20"/>
-      <c r="L9" s="29"/>
-      <c r="M9" s="29"/>
       <c r="P9" s="21"/>
-      <c r="S9" s="45"/>
-      <c r="T9" s="21"/>
-      <c r="Y9" s="47"/>
-    </row>
-    <row r="10" spans="1:26" s="18" customFormat="1" ht="15.75">
+      <c r="T9" s="45"/>
+      <c r="U9" s="21"/>
+      <c r="Z9" s="47"/>
+    </row>
+    <row r="10" spans="1:27" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D10" s="19"/>
       <c r="G10" s="47"/>
       <c r="H10" s="59"/>
       <c r="J10" s="20"/>
-      <c r="L10" s="29"/>
-      <c r="M10" s="29"/>
       <c r="P10" s="21"/>
-      <c r="S10" s="45"/>
-      <c r="T10" s="21"/>
-      <c r="Y10" s="47"/>
-    </row>
-    <row r="11" spans="1:26" s="18" customFormat="1" ht="15.75">
+      <c r="T10" s="45"/>
+      <c r="U10" s="21"/>
+      <c r="Z10" s="47"/>
+    </row>
+    <row r="11" spans="1:27" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D11" s="19"/>
       <c r="G11" s="47"/>
       <c r="H11" s="59"/>
-      <c r="I11" s="27"/>
       <c r="J11" s="20"/>
-      <c r="L11" s="29"/>
-      <c r="M11" s="29"/>
       <c r="P11" s="21"/>
-      <c r="S11" s="45"/>
-      <c r="T11" s="21"/>
-      <c r="Y11" s="47"/>
-    </row>
-    <row r="12" spans="1:26" s="18" customFormat="1" ht="15.75">
+      <c r="T11" s="45"/>
+      <c r="U11" s="21"/>
+      <c r="Z11" s="47"/>
+    </row>
+    <row r="12" spans="1:27" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D12" s="19"/>
       <c r="G12" s="47"/>
       <c r="H12" s="59"/>
-      <c r="I12" s="27"/>
       <c r="J12" s="20"/>
-      <c r="L12" s="29"/>
-      <c r="M12" s="29"/>
       <c r="P12" s="21"/>
-      <c r="S12" s="45"/>
-      <c r="T12" s="21"/>
-      <c r="Y12" s="49"/>
-    </row>
-    <row r="13" spans="1:26" s="18" customFormat="1" ht="15.75">
+      <c r="T12" s="45"/>
+      <c r="U12" s="21"/>
+      <c r="Z12" s="49"/>
+    </row>
+    <row r="13" spans="1:27" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D13" s="19"/>
       <c r="G13" s="47"/>
       <c r="H13" s="59"/>
       <c r="J13" s="20"/>
-      <c r="L13" s="29"/>
-      <c r="M13" s="29"/>
       <c r="P13" s="21"/>
-      <c r="S13" s="45"/>
-      <c r="T13" s="21"/>
-      <c r="Y13" s="47"/>
-    </row>
-    <row r="14" spans="1:26" s="18" customFormat="1" ht="15.75">
+      <c r="T13" s="45"/>
+      <c r="U13" s="21"/>
+      <c r="Z13" s="47"/>
+    </row>
+    <row r="14" spans="1:27" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D14" s="19"/>
       <c r="G14" s="47"/>
       <c r="H14" s="59"/>
       <c r="J14" s="20"/>
-      <c r="L14" s="29"/>
-      <c r="M14" s="29"/>
       <c r="P14" s="21"/>
-      <c r="S14" s="45"/>
-      <c r="T14" s="21"/>
-      <c r="Y14" s="47"/>
-    </row>
-    <row r="15" spans="1:26" s="18" customFormat="1" ht="15.75">
+      <c r="T14" s="45"/>
+      <c r="U14" s="21"/>
+      <c r="Z14" s="47"/>
+    </row>
+    <row r="15" spans="1:27" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D15" s="19"/>
       <c r="G15" s="47"/>
       <c r="H15" s="59"/>
       <c r="J15" s="20"/>
-      <c r="L15" s="29"/>
-      <c r="M15" s="29"/>
       <c r="P15" s="21"/>
-      <c r="S15" s="45"/>
-      <c r="T15" s="21"/>
-      <c r="Y15" s="47"/>
-    </row>
-    <row r="16" spans="1:26" s="18" customFormat="1" ht="15.75">
+      <c r="T15" s="45"/>
+      <c r="U15" s="21"/>
+      <c r="Z15" s="47"/>
+    </row>
+    <row r="16" spans="1:27" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D16" s="19"/>
       <c r="G16" s="47"/>
       <c r="H16" s="59"/>
       <c r="J16" s="20"/>
-      <c r="L16" s="29"/>
-      <c r="M16" s="29"/>
       <c r="P16" s="21"/>
-      <c r="S16" s="45"/>
-      <c r="T16" s="21"/>
-      <c r="Y16" s="47"/>
-    </row>
-    <row r="17" spans="4:25" s="18" customFormat="1" ht="15.75">
+      <c r="T16" s="45"/>
+      <c r="U16" s="21"/>
+      <c r="Z16" s="47"/>
+    </row>
+    <row r="17" spans="4:26" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D17" s="19"/>
       <c r="G17" s="47"/>
       <c r="H17" s="59"/>
       <c r="J17" s="20"/>
-      <c r="L17" s="29"/>
-      <c r="M17" s="29"/>
       <c r="P17" s="21"/>
-      <c r="S17" s="45"/>
-      <c r="T17" s="21"/>
-      <c r="Y17" s="47"/>
-    </row>
-    <row r="18" spans="4:25" s="18" customFormat="1" ht="15.75">
+      <c r="T17" s="45"/>
+      <c r="U17" s="21"/>
+      <c r="Z17" s="47"/>
+    </row>
+    <row r="18" spans="4:26" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D18" s="19"/>
       <c r="G18" s="47"/>
       <c r="H18" s="59"/>
       <c r="J18" s="20"/>
-      <c r="L18" s="29"/>
-      <c r="M18" s="29"/>
       <c r="P18" s="21"/>
-      <c r="S18" s="45"/>
-      <c r="T18" s="21"/>
-      <c r="Y18" s="47"/>
-    </row>
-    <row r="19" spans="4:25" s="18" customFormat="1" ht="15.75">
+      <c r="T18" s="45"/>
+      <c r="U18" s="21"/>
+      <c r="Z18" s="47"/>
+    </row>
+    <row r="19" spans="4:26" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D19" s="19"/>
       <c r="G19" s="47"/>
       <c r="H19" s="59"/>
       <c r="J19" s="20"/>
-      <c r="L19" s="29"/>
-      <c r="M19" s="29"/>
       <c r="P19" s="21"/>
-      <c r="S19" s="45"/>
-      <c r="T19" s="21"/>
-      <c r="Y19" s="47"/>
-    </row>
-    <row r="20" spans="4:25" s="18" customFormat="1" ht="15.75">
+      <c r="T19" s="45"/>
+      <c r="U19" s="21"/>
+      <c r="Z19" s="47"/>
+    </row>
+    <row r="20" spans="4:26" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D20" s="19"/>
       <c r="G20" s="47"/>
       <c r="H20" s="59"/>
       <c r="J20" s="20"/>
-      <c r="L20" s="29"/>
-      <c r="M20" s="29"/>
       <c r="P20" s="21"/>
-      <c r="S20" s="45"/>
-      <c r="T20" s="21"/>
-      <c r="Y20" s="47"/>
-    </row>
-    <row r="21" spans="4:25" s="18" customFormat="1" ht="15.75">
+      <c r="T20" s="45"/>
+      <c r="U20" s="21"/>
+      <c r="Z20" s="47"/>
+    </row>
+    <row r="21" spans="4:26" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D21" s="19"/>
       <c r="G21" s="47"/>
       <c r="H21" s="59"/>
       <c r="J21" s="20"/>
-      <c r="L21" s="29"/>
-      <c r="M21" s="29"/>
       <c r="P21" s="21"/>
-      <c r="S21" s="45"/>
-      <c r="T21" s="21"/>
-      <c r="Y21" s="47"/>
-    </row>
-    <row r="22" spans="4:25" s="18" customFormat="1" ht="15.75">
+      <c r="T21" s="45"/>
+      <c r="U21" s="21"/>
+      <c r="Z21" s="47"/>
+    </row>
+    <row r="22" spans="4:26" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D22" s="19"/>
       <c r="G22" s="47"/>
       <c r="H22" s="59"/>
       <c r="J22" s="20"/>
-      <c r="L22" s="29"/>
-      <c r="M22" s="29"/>
       <c r="P22" s="21"/>
-      <c r="S22" s="45"/>
-      <c r="T22" s="21"/>
-      <c r="Y22" s="47"/>
-    </row>
-    <row r="23" spans="4:25" s="18" customFormat="1" ht="15.75">
+      <c r="T22" s="45"/>
+      <c r="U22" s="21"/>
+      <c r="Z22" s="47"/>
+    </row>
+    <row r="23" spans="4:26" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D23" s="19"/>
       <c r="G23" s="47"/>
       <c r="H23" s="59"/>
       <c r="J23" s="20"/>
-      <c r="L23" s="29"/>
-      <c r="M23" s="29"/>
       <c r="P23" s="21"/>
-      <c r="S23" s="45"/>
-      <c r="T23" s="21"/>
-      <c r="Y23" s="47"/>
-    </row>
-    <row r="24" spans="4:25" s="18" customFormat="1" ht="15.75">
+      <c r="T23" s="45"/>
+      <c r="U23" s="21"/>
+      <c r="Z23" s="47"/>
+    </row>
+    <row r="24" spans="4:26" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D24" s="19"/>
       <c r="G24" s="47"/>
       <c r="H24" s="59"/>
       <c r="J24" s="20"/>
-      <c r="L24" s="29"/>
-      <c r="M24" s="29"/>
       <c r="P24" s="21"/>
-      <c r="S24" s="45"/>
-      <c r="T24" s="21"/>
-      <c r="Y24" s="47"/>
-    </row>
-    <row r="25" spans="4:25" s="18" customFormat="1" ht="15.75">
+      <c r="T24" s="45"/>
+      <c r="U24" s="21"/>
+      <c r="Z24" s="47"/>
+    </row>
+    <row r="25" spans="4:26" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D25" s="19"/>
       <c r="G25" s="47"/>
       <c r="H25" s="59"/>
       <c r="J25" s="20"/>
-      <c r="L25" s="29"/>
-      <c r="M25" s="29"/>
       <c r="P25" s="21"/>
-      <c r="S25" s="45"/>
-      <c r="T25" s="21"/>
-      <c r="Y25" s="47"/>
-    </row>
-    <row r="26" spans="4:25" s="18" customFormat="1" ht="15.75">
+      <c r="T25" s="45"/>
+      <c r="U25" s="21"/>
+      <c r="Z25" s="47"/>
+    </row>
+    <row r="26" spans="4:26" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D26" s="19"/>
       <c r="G26" s="47"/>
       <c r="H26" s="59"/>
       <c r="J26" s="20"/>
-      <c r="L26" s="29"/>
-      <c r="M26" s="29"/>
       <c r="P26" s="21"/>
-      <c r="S26" s="45"/>
-      <c r="T26" s="21"/>
-      <c r="Y26" s="47"/>
-    </row>
-    <row r="27" spans="4:25" s="18" customFormat="1" ht="15.75">
+      <c r="T26" s="45"/>
+      <c r="U26" s="21"/>
+      <c r="Z26" s="47"/>
+    </row>
+    <row r="27" spans="4:26" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D27" s="19"/>
       <c r="G27" s="47"/>
       <c r="H27" s="59"/>
       <c r="J27" s="20"/>
-      <c r="L27" s="29"/>
-      <c r="M27" s="29"/>
       <c r="P27" s="21"/>
-      <c r="S27" s="45"/>
-      <c r="T27" s="21"/>
-      <c r="Y27" s="47"/>
-    </row>
-    <row r="28" spans="4:25" s="18" customFormat="1" ht="15.75">
+      <c r="T27" s="45"/>
+      <c r="U27" s="21"/>
+      <c r="Z27" s="47"/>
+    </row>
+    <row r="28" spans="4:26" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D28" s="19"/>
       <c r="G28" s="47"/>
       <c r="H28" s="59"/>
       <c r="J28" s="20"/>
-      <c r="L28" s="29"/>
-      <c r="M28" s="29"/>
       <c r="P28" s="21"/>
-      <c r="S28" s="45"/>
-      <c r="T28" s="21"/>
-      <c r="Y28" s="47"/>
-    </row>
-    <row r="29" spans="4:25" s="18" customFormat="1" ht="15.75">
+      <c r="T28" s="45"/>
+      <c r="U28" s="21"/>
+      <c r="Z28" s="47"/>
+    </row>
+    <row r="29" spans="4:26" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D29" s="19"/>
       <c r="G29" s="47"/>
       <c r="H29" s="59"/>
       <c r="J29" s="20"/>
-      <c r="L29" s="29"/>
-      <c r="M29" s="29"/>
       <c r="P29" s="21"/>
-      <c r="S29" s="45"/>
-      <c r="T29" s="21"/>
-      <c r="Y29" s="47"/>
-    </row>
-    <row r="30" spans="4:25" s="18" customFormat="1" ht="15.75">
+      <c r="T29" s="45"/>
+      <c r="U29" s="21"/>
+      <c r="Z29" s="47"/>
+    </row>
+    <row r="30" spans="4:26" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D30" s="19"/>
       <c r="G30" s="47"/>
       <c r="H30" s="59"/>
       <c r="J30" s="20"/>
-      <c r="L30" s="29"/>
-      <c r="M30" s="29"/>
       <c r="P30" s="21"/>
-      <c r="S30" s="45"/>
-      <c r="T30" s="21"/>
-      <c r="Y30" s="47"/>
-    </row>
-    <row r="31" spans="4:25" s="18" customFormat="1" ht="15.75">
+      <c r="T30" s="45"/>
+      <c r="U30" s="21"/>
+      <c r="Z30" s="47"/>
+    </row>
+    <row r="31" spans="4:26" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D31" s="19"/>
       <c r="G31" s="47"/>
       <c r="H31" s="59"/>
       <c r="J31" s="20"/>
-      <c r="L31" s="29"/>
-      <c r="M31" s="29"/>
       <c r="P31" s="21"/>
-      <c r="S31" s="45"/>
-      <c r="T31" s="21"/>
-      <c r="Y31" s="47"/>
-    </row>
-    <row r="32" spans="4:25" s="18" customFormat="1" ht="15.75">
+      <c r="T31" s="45"/>
+      <c r="U31" s="21"/>
+      <c r="Z31" s="47"/>
+    </row>
+    <row r="32" spans="4:26" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D32" s="19"/>
       <c r="G32" s="47"/>
       <c r="H32" s="59"/>
       <c r="J32" s="20"/>
-      <c r="L32" s="29"/>
-      <c r="M32" s="29"/>
       <c r="P32" s="21"/>
-      <c r="S32" s="45"/>
-      <c r="T32" s="21"/>
-      <c r="Y32" s="47"/>
-    </row>
-    <row r="33" spans="4:25" s="18" customFormat="1" ht="15.75">
+      <c r="T32" s="45"/>
+      <c r="U32" s="21"/>
+      <c r="Z32" s="47"/>
+    </row>
+    <row r="33" spans="4:26" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D33" s="19"/>
       <c r="G33" s="47"/>
       <c r="H33" s="59"/>
       <c r="J33" s="20"/>
-      <c r="L33" s="29"/>
-      <c r="M33" s="29"/>
       <c r="P33" s="21"/>
-      <c r="S33" s="45"/>
-      <c r="T33" s="21"/>
-      <c r="Y33" s="47"/>
-    </row>
-    <row r="34" spans="4:25" s="18" customFormat="1" ht="15.75">
+      <c r="T33" s="45"/>
+      <c r="U33" s="21"/>
+      <c r="Z33" s="47"/>
+    </row>
+    <row r="34" spans="4:26" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D34" s="19"/>
       <c r="G34" s="47"/>
       <c r="H34" s="59"/>
       <c r="J34" s="20"/>
-      <c r="L34" s="29"/>
-      <c r="M34" s="29"/>
       <c r="P34" s="21"/>
-      <c r="S34" s="45"/>
-      <c r="T34" s="21"/>
-      <c r="Y34" s="47"/>
-    </row>
-    <row r="35" spans="4:25" s="18" customFormat="1" ht="15.75">
+      <c r="T34" s="45"/>
+      <c r="U34" s="21"/>
+      <c r="Z34" s="47"/>
+    </row>
+    <row r="35" spans="4:26" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D35" s="19"/>
       <c r="G35" s="47"/>
       <c r="H35" s="59"/>
       <c r="J35" s="20"/>
-      <c r="L35" s="29"/>
-      <c r="M35" s="29"/>
       <c r="P35" s="21"/>
-      <c r="S35" s="45"/>
-      <c r="T35" s="21"/>
-      <c r="Y35" s="47"/>
-    </row>
-    <row r="36" spans="4:25" s="18" customFormat="1" ht="15.75">
+      <c r="T35" s="45"/>
+      <c r="U35" s="21"/>
+      <c r="Z35" s="47"/>
+    </row>
+    <row r="36" spans="4:26" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D36" s="19"/>
       <c r="G36" s="47"/>
       <c r="H36" s="59"/>
       <c r="J36" s="20"/>
-      <c r="L36" s="29"/>
-      <c r="M36" s="29"/>
       <c r="P36" s="21"/>
-      <c r="S36" s="45"/>
-      <c r="T36" s="21"/>
-      <c r="Y36" s="47"/>
-    </row>
-    <row r="37" spans="4:25" s="18" customFormat="1" ht="15.75">
+      <c r="T36" s="45"/>
+      <c r="U36" s="21"/>
+      <c r="Z36" s="47"/>
+    </row>
+    <row r="37" spans="4:26" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D37" s="19"/>
       <c r="G37" s="47"/>
       <c r="H37" s="59"/>
       <c r="J37" s="20"/>
-      <c r="L37" s="29"/>
-      <c r="M37" s="29"/>
       <c r="P37" s="21"/>
-      <c r="S37" s="45"/>
-      <c r="T37" s="21"/>
-      <c r="Y37" s="47"/>
-    </row>
-    <row r="38" spans="4:25" s="18" customFormat="1" ht="15.75">
+      <c r="T37" s="45"/>
+      <c r="U37" s="21"/>
+      <c r="Z37" s="47"/>
+    </row>
+    <row r="38" spans="4:26" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D38" s="19"/>
       <c r="G38" s="47"/>
       <c r="H38" s="59"/>
       <c r="J38" s="20"/>
-      <c r="L38" s="29"/>
-      <c r="M38" s="29"/>
       <c r="P38" s="21"/>
-      <c r="S38" s="45"/>
-      <c r="T38" s="21"/>
-      <c r="Y38" s="47"/>
-    </row>
-    <row r="39" spans="4:25" s="18" customFormat="1" ht="15.75">
+      <c r="T38" s="45"/>
+      <c r="U38" s="21"/>
+      <c r="Z38" s="47"/>
+    </row>
+    <row r="39" spans="4:26" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D39" s="19"/>
       <c r="G39" s="47"/>
       <c r="H39" s="59"/>
       <c r="J39" s="20"/>
-      <c r="L39" s="29"/>
-      <c r="M39" s="29"/>
       <c r="P39" s="21"/>
-      <c r="S39" s="45"/>
-      <c r="T39" s="21"/>
-      <c r="Y39" s="47"/>
-    </row>
-    <row r="40" spans="4:25" s="18" customFormat="1" ht="15.75">
+      <c r="T39" s="45"/>
+      <c r="U39" s="21"/>
+      <c r="Z39" s="47"/>
+    </row>
+    <row r="40" spans="4:26" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D40" s="19"/>
       <c r="G40" s="47"/>
       <c r="H40" s="59"/>
       <c r="J40" s="20"/>
-      <c r="L40" s="29"/>
-      <c r="M40" s="29"/>
       <c r="P40" s="21"/>
-      <c r="S40" s="45"/>
-      <c r="T40" s="21"/>
-      <c r="Y40" s="47"/>
-    </row>
-    <row r="41" spans="4:25" s="18" customFormat="1" ht="15.75">
+      <c r="T40" s="45"/>
+      <c r="U40" s="21"/>
+      <c r="Z40" s="47"/>
+    </row>
+    <row r="41" spans="4:26" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D41" s="19"/>
       <c r="G41" s="47"/>
       <c r="H41" s="59"/>
       <c r="J41" s="20"/>
-      <c r="L41" s="29"/>
-      <c r="M41" s="29"/>
       <c r="P41" s="21"/>
-      <c r="S41" s="45"/>
-      <c r="T41" s="21"/>
-      <c r="Y41" s="47"/>
-    </row>
-    <row r="42" spans="4:25" s="18" customFormat="1" ht="15.75">
+      <c r="T41" s="45"/>
+      <c r="U41" s="21"/>
+      <c r="Z41" s="47"/>
+    </row>
+    <row r="42" spans="4:26" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D42" s="19"/>
       <c r="G42" s="47"/>
       <c r="H42" s="59"/>
       <c r="J42" s="20"/>
-      <c r="L42" s="29"/>
-      <c r="M42" s="29"/>
       <c r="P42" s="21"/>
-      <c r="S42" s="45"/>
-      <c r="T42" s="21"/>
-      <c r="Y42" s="47"/>
-    </row>
-    <row r="43" spans="4:25" s="18" customFormat="1" ht="15.75">
+      <c r="T42" s="45"/>
+      <c r="U42" s="21"/>
+      <c r="Z42" s="47"/>
+    </row>
+    <row r="43" spans="4:26" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D43" s="19"/>
       <c r="G43" s="47"/>
       <c r="H43" s="59"/>
       <c r="J43" s="20"/>
-      <c r="L43" s="29"/>
-      <c r="M43" s="29"/>
       <c r="P43" s="21"/>
-      <c r="S43" s="45"/>
-      <c r="T43" s="21"/>
-      <c r="Y43" s="47"/>
-    </row>
-    <row r="44" spans="4:25" s="18" customFormat="1" ht="15.75">
+      <c r="T43" s="45"/>
+      <c r="U43" s="21"/>
+      <c r="Z43" s="47"/>
+    </row>
+    <row r="44" spans="4:26" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D44" s="19"/>
       <c r="G44" s="47"/>
       <c r="H44" s="59"/>
       <c r="J44" s="20"/>
-      <c r="L44" s="29"/>
-      <c r="M44" s="29"/>
       <c r="P44" s="21"/>
-      <c r="S44" s="45"/>
-      <c r="T44" s="21"/>
-      <c r="Y44" s="47"/>
-    </row>
-    <row r="45" spans="4:25" s="18" customFormat="1" ht="15.75">
+      <c r="T44" s="45"/>
+      <c r="U44" s="21"/>
+      <c r="Z44" s="47"/>
+    </row>
+    <row r="45" spans="4:26" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D45" s="19"/>
       <c r="G45" s="47"/>
       <c r="H45" s="59"/>
       <c r="J45" s="20"/>
-      <c r="L45" s="29"/>
-      <c r="M45" s="29"/>
       <c r="P45" s="21"/>
-      <c r="S45" s="45"/>
-      <c r="T45" s="21"/>
-      <c r="Y45" s="47"/>
-    </row>
-    <row r="46" spans="4:25" s="18" customFormat="1" ht="15.75">
+      <c r="T45" s="45"/>
+      <c r="U45" s="21"/>
+      <c r="Z45" s="47"/>
+    </row>
+    <row r="46" spans="4:26" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D46" s="19"/>
       <c r="G46" s="47"/>
       <c r="H46" s="59"/>
       <c r="J46" s="20"/>
-      <c r="L46" s="29"/>
-      <c r="M46" s="29"/>
       <c r="P46" s="21"/>
-      <c r="S46" s="45"/>
-      <c r="T46" s="21"/>
-      <c r="Y46" s="47"/>
-    </row>
-    <row r="47" spans="4:25" s="18" customFormat="1" ht="15.75">
+      <c r="T46" s="45"/>
+      <c r="U46" s="21"/>
+      <c r="Z46" s="47"/>
+    </row>
+    <row r="47" spans="4:26" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D47" s="19"/>
       <c r="G47" s="47"/>
       <c r="H47" s="59"/>
       <c r="J47" s="20"/>
-      <c r="L47" s="29"/>
-      <c r="M47" s="29"/>
       <c r="P47" s="21"/>
-      <c r="S47" s="45"/>
-      <c r="T47" s="21"/>
-      <c r="Y47" s="47"/>
-    </row>
-    <row r="48" spans="4:25" s="18" customFormat="1" ht="15.75">
+      <c r="T47" s="45"/>
+      <c r="U47" s="21"/>
+      <c r="Z47" s="47"/>
+    </row>
+    <row r="48" spans="4:26" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D48" s="19"/>
       <c r="G48" s="47"/>
       <c r="H48" s="59"/>
       <c r="J48" s="20"/>
-      <c r="L48" s="29"/>
-      <c r="M48" s="29"/>
       <c r="P48" s="21"/>
-      <c r="S48" s="45"/>
-      <c r="T48" s="21"/>
-      <c r="Y48" s="47"/>
-    </row>
-    <row r="49" spans="4:25" s="18" customFormat="1" ht="15.75">
+      <c r="T48" s="45"/>
+      <c r="U48" s="21"/>
+      <c r="Z48" s="47"/>
+    </row>
+    <row r="49" spans="4:26" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D49" s="19"/>
       <c r="G49" s="47"/>
       <c r="H49" s="59"/>
       <c r="J49" s="20"/>
-      <c r="L49" s="29"/>
-      <c r="M49" s="29"/>
       <c r="P49" s="21"/>
-      <c r="S49" s="45"/>
-      <c r="T49" s="21"/>
-      <c r="Y49" s="47"/>
-    </row>
-    <row r="50" spans="4:25" s="18" customFormat="1" ht="15.75">
+      <c r="T49" s="45"/>
+      <c r="U49" s="21"/>
+      <c r="Z49" s="47"/>
+    </row>
+    <row r="50" spans="4:26" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D50" s="19"/>
       <c r="G50" s="47"/>
       <c r="H50" s="59"/>
       <c r="J50" s="20"/>
-      <c r="L50" s="29"/>
-      <c r="M50" s="29"/>
       <c r="P50" s="21"/>
-      <c r="S50" s="45"/>
-      <c r="T50" s="21"/>
-      <c r="Y50" s="47"/>
-    </row>
-    <row r="51" spans="4:25" s="18" customFormat="1" ht="15.75">
+      <c r="T50" s="45"/>
+      <c r="U50" s="21"/>
+      <c r="Z50" s="47"/>
+    </row>
+    <row r="51" spans="4:26" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D51" s="19"/>
       <c r="G51" s="47"/>
       <c r="H51" s="59"/>
       <c r="J51" s="20"/>
-      <c r="L51" s="29"/>
-      <c r="M51" s="29"/>
       <c r="P51" s="21"/>
-      <c r="S51" s="45"/>
-      <c r="T51" s="21"/>
-      <c r="Y51" s="47"/>
-    </row>
-    <row r="52" spans="4:25" s="18" customFormat="1" ht="15.75">
+      <c r="T51" s="45"/>
+      <c r="U51" s="21"/>
+      <c r="Z51" s="47"/>
+    </row>
+    <row r="52" spans="4:26" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D52" s="19"/>
       <c r="G52" s="47"/>
       <c r="H52" s="59"/>
       <c r="J52" s="20"/>
-      <c r="L52" s="29"/>
-      <c r="M52" s="29"/>
       <c r="P52" s="21"/>
-      <c r="S52" s="45"/>
-      <c r="T52" s="21"/>
-      <c r="Y52" s="47"/>
-    </row>
-    <row r="53" spans="4:25" s="18" customFormat="1" ht="15.75">
+      <c r="T52" s="45"/>
+      <c r="U52" s="21"/>
+      <c r="Z52" s="47"/>
+    </row>
+    <row r="53" spans="4:26" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D53" s="19"/>
       <c r="G53" s="47"/>
       <c r="H53" s="59"/>
       <c r="J53" s="20"/>
-      <c r="L53" s="29"/>
-      <c r="M53" s="29"/>
       <c r="P53" s="21"/>
-      <c r="S53" s="45"/>
-      <c r="T53" s="21"/>
-      <c r="Y53" s="47"/>
-    </row>
-    <row r="54" spans="4:25">
+      <c r="T53" s="45"/>
+      <c r="U53" s="21"/>
+      <c r="Z53" s="47"/>
+    </row>
+    <row r="54" spans="4:26" x14ac:dyDescent="0.25">
       <c r="G54" s="48"/>
       <c r="H54" s="59"/>
       <c r="J54" s="31"/>
       <c r="P54" s="21"/>
-      <c r="S54" s="46"/>
-    </row>
-    <row r="55" spans="4:25">
+      <c r="T54" s="46"/>
+    </row>
+    <row r="55" spans="4:26" x14ac:dyDescent="0.25">
       <c r="G55" s="48"/>
       <c r="H55" s="59"/>
       <c r="J55" s="31"/>
       <c r="P55" s="21"/>
-      <c r="S55" s="46"/>
-    </row>
-    <row r="56" spans="4:25">
+      <c r="T55" s="46"/>
+    </row>
+    <row r="56" spans="4:26" x14ac:dyDescent="0.25">
       <c r="G56" s="48"/>
       <c r="H56" s="59"/>
       <c r="J56" s="31"/>
       <c r="P56" s="21"/>
-      <c r="S56" s="46"/>
-    </row>
-    <row r="57" spans="4:25">
+      <c r="T56" s="46"/>
+    </row>
+    <row r="57" spans="4:26" x14ac:dyDescent="0.25">
       <c r="G57" s="48"/>
       <c r="H57" s="59"/>
       <c r="J57" s="31"/>
       <c r="P57" s="21"/>
-      <c r="S57" s="46"/>
-    </row>
-    <row r="58" spans="4:25">
+      <c r="T57" s="46"/>
+    </row>
+    <row r="58" spans="4:26" x14ac:dyDescent="0.25">
       <c r="G58" s="48"/>
       <c r="H58" s="59"/>
       <c r="J58" s="31"/>
       <c r="P58" s="21"/>
-      <c r="S58" s="46"/>
-    </row>
-    <row r="59" spans="4:25">
+      <c r="T58" s="46"/>
+    </row>
+    <row r="59" spans="4:26" x14ac:dyDescent="0.25">
       <c r="G59" s="48"/>
       <c r="H59" s="59"/>
       <c r="J59" s="31"/>
       <c r="P59" s="21"/>
-      <c r="S59" s="46"/>
-    </row>
-    <row r="60" spans="4:25">
+      <c r="T59" s="46"/>
+    </row>
+    <row r="60" spans="4:26" x14ac:dyDescent="0.25">
       <c r="G60" s="48"/>
       <c r="H60" s="59"/>
       <c r="J60" s="31"/>
       <c r="P60" s="21"/>
-      <c r="S60" s="46"/>
-    </row>
-    <row r="61" spans="4:25">
+      <c r="T60" s="46"/>
+    </row>
+    <row r="61" spans="4:26" x14ac:dyDescent="0.25">
       <c r="G61" s="48"/>
       <c r="H61" s="59"/>
       <c r="J61" s="31"/>
       <c r="P61" s="21"/>
-      <c r="S61" s="46"/>
-    </row>
-    <row r="62" spans="4:25">
+      <c r="T61" s="46"/>
+    </row>
+    <row r="62" spans="4:26" x14ac:dyDescent="0.25">
       <c r="G62" s="48"/>
       <c r="H62" s="59"/>
       <c r="J62" s="31"/>
       <c r="P62" s="21"/>
-      <c r="S62" s="46"/>
-    </row>
-    <row r="63" spans="4:25">
+      <c r="T62" s="46"/>
+    </row>
+    <row r="63" spans="4:26" x14ac:dyDescent="0.25">
       <c r="G63" s="48"/>
       <c r="H63" s="59"/>
       <c r="J63" s="31"/>
       <c r="P63" s="21"/>
-      <c r="S63" s="46"/>
-    </row>
-    <row r="64" spans="4:25">
+      <c r="T63" s="46"/>
+    </row>
+    <row r="64" spans="4:26" x14ac:dyDescent="0.25">
       <c r="G64" s="48"/>
       <c r="H64" s="59"/>
       <c r="J64" s="31"/>
       <c r="P64" s="21"/>
-      <c r="S64" s="46"/>
-    </row>
-    <row r="65" spans="7:19">
+      <c r="T64" s="46"/>
+    </row>
+    <row r="65" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G65" s="48"/>
       <c r="H65" s="59"/>
       <c r="J65" s="31"/>
       <c r="P65" s="21"/>
-      <c r="S65" s="46"/>
-    </row>
-    <row r="66" spans="7:19">
+      <c r="T65" s="46"/>
+    </row>
+    <row r="66" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G66" s="48"/>
       <c r="H66" s="59"/>
       <c r="J66" s="31"/>
       <c r="P66" s="21"/>
-      <c r="S66" s="46"/>
-    </row>
-    <row r="67" spans="7:19">
+      <c r="T66" s="46"/>
+    </row>
+    <row r="67" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G67" s="48"/>
       <c r="H67" s="59"/>
       <c r="J67" s="31"/>
       <c r="P67" s="21"/>
-      <c r="S67" s="46"/>
-    </row>
-    <row r="68" spans="7:19">
+      <c r="T67" s="46"/>
+    </row>
+    <row r="68" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G68" s="48"/>
       <c r="H68" s="59"/>
       <c r="J68" s="31"/>
       <c r="P68" s="21"/>
-      <c r="S68" s="46"/>
-    </row>
-    <row r="69" spans="7:19">
+      <c r="T68" s="46"/>
+    </row>
+    <row r="69" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G69" s="48"/>
       <c r="H69" s="59"/>
       <c r="J69" s="31"/>
       <c r="P69" s="21"/>
-      <c r="S69" s="46"/>
-    </row>
-    <row r="70" spans="7:19">
+      <c r="T69" s="46"/>
+    </row>
+    <row r="70" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G70" s="48"/>
       <c r="H70" s="59"/>
       <c r="J70" s="31"/>
       <c r="P70" s="21"/>
-      <c r="S70" s="46"/>
-    </row>
-    <row r="71" spans="7:19">
+      <c r="T70" s="46"/>
+    </row>
+    <row r="71" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G71" s="48"/>
       <c r="H71" s="59"/>
       <c r="J71" s="31"/>
       <c r="P71" s="21"/>
-      <c r="S71" s="46"/>
-    </row>
-    <row r="72" spans="7:19">
+      <c r="T71" s="46"/>
+    </row>
+    <row r="72" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G72" s="48"/>
       <c r="H72" s="59"/>
       <c r="J72" s="31"/>
       <c r="P72" s="21"/>
-      <c r="S72" s="46"/>
-    </row>
-    <row r="73" spans="7:19">
+      <c r="T72" s="46"/>
+    </row>
+    <row r="73" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G73" s="48"/>
       <c r="H73" s="59"/>
       <c r="J73" s="31"/>
       <c r="P73" s="21"/>
-      <c r="S73" s="46"/>
-    </row>
-    <row r="74" spans="7:19">
+      <c r="T73" s="46"/>
+    </row>
+    <row r="74" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G74" s="48"/>
       <c r="H74" s="59"/>
       <c r="J74" s="31"/>
       <c r="P74" s="21"/>
-      <c r="S74" s="46"/>
-    </row>
-    <row r="75" spans="7:19">
+      <c r="T74" s="46"/>
+    </row>
+    <row r="75" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G75" s="48"/>
       <c r="H75" s="59"/>
       <c r="J75" s="31"/>
       <c r="P75" s="21"/>
-      <c r="S75" s="46"/>
-    </row>
-    <row r="76" spans="7:19">
+      <c r="T75" s="46"/>
+    </row>
+    <row r="76" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G76" s="48"/>
       <c r="H76" s="59"/>
       <c r="J76" s="31"/>
       <c r="P76" s="21"/>
-      <c r="S76" s="46"/>
-    </row>
-    <row r="77" spans="7:19">
+      <c r="T76" s="46"/>
+    </row>
+    <row r="77" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G77" s="48"/>
       <c r="H77" s="59"/>
       <c r="J77" s="31"/>
       <c r="P77" s="21"/>
-      <c r="S77" s="46"/>
-    </row>
-    <row r="78" spans="7:19">
+      <c r="T77" s="46"/>
+    </row>
+    <row r="78" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G78" s="48"/>
       <c r="H78" s="59"/>
       <c r="J78" s="31"/>
       <c r="P78" s="21"/>
-      <c r="S78" s="46"/>
-    </row>
-    <row r="79" spans="7:19">
+      <c r="T78" s="46"/>
+    </row>
+    <row r="79" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G79" s="48"/>
       <c r="H79" s="59"/>
       <c r="J79" s="31"/>
       <c r="P79" s="21"/>
-      <c r="S79" s="46"/>
-    </row>
-    <row r="80" spans="7:19">
+      <c r="T79" s="46"/>
+    </row>
+    <row r="80" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G80" s="48"/>
       <c r="H80" s="59"/>
       <c r="J80" s="31"/>
       <c r="P80" s="21"/>
-      <c r="S80" s="46"/>
-    </row>
-    <row r="81" spans="7:19">
+      <c r="T80" s="46"/>
+    </row>
+    <row r="81" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G81" s="48"/>
       <c r="H81" s="59"/>
       <c r="J81" s="31"/>
       <c r="P81" s="21"/>
-      <c r="S81" s="46"/>
-    </row>
-    <row r="82" spans="7:19">
+      <c r="T81" s="46"/>
+    </row>
+    <row r="82" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G82" s="48"/>
       <c r="H82" s="59"/>
       <c r="J82" s="31"/>
       <c r="P82" s="21"/>
-      <c r="S82" s="46"/>
-    </row>
-    <row r="83" spans="7:19">
+      <c r="T82" s="46"/>
+    </row>
+    <row r="83" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G83" s="48"/>
       <c r="H83" s="59"/>
       <c r="J83" s="31"/>
       <c r="P83" s="21"/>
-      <c r="S83" s="46"/>
-    </row>
-    <row r="84" spans="7:19">
+      <c r="T83" s="46"/>
+    </row>
+    <row r="84" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G84" s="48"/>
       <c r="H84" s="59"/>
       <c r="J84" s="31"/>
       <c r="P84" s="21"/>
-      <c r="S84" s="46"/>
-    </row>
-    <row r="85" spans="7:19">
+      <c r="T84" s="46"/>
+    </row>
+    <row r="85" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G85" s="48"/>
       <c r="H85" s="59"/>
       <c r="J85" s="31"/>
       <c r="P85" s="21"/>
-      <c r="S85" s="46"/>
-    </row>
-    <row r="86" spans="7:19">
+      <c r="T85" s="46"/>
+    </row>
+    <row r="86" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G86" s="48"/>
       <c r="H86" s="59"/>
       <c r="J86" s="31"/>
       <c r="P86" s="21"/>
-      <c r="S86" s="46"/>
-    </row>
-    <row r="87" spans="7:19">
+      <c r="T86" s="46"/>
+    </row>
+    <row r="87" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G87" s="48"/>
       <c r="H87" s="59"/>
       <c r="J87" s="31"/>
       <c r="P87" s="21"/>
-      <c r="S87" s="46"/>
-    </row>
-    <row r="88" spans="7:19">
+      <c r="T87" s="46"/>
+    </row>
+    <row r="88" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G88" s="48"/>
       <c r="H88" s="59"/>
       <c r="J88" s="31"/>
       <c r="P88" s="21"/>
-      <c r="S88" s="46"/>
-    </row>
-    <row r="89" spans="7:19">
+      <c r="T88" s="46"/>
+    </row>
+    <row r="89" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G89" s="48"/>
       <c r="H89" s="59"/>
       <c r="J89" s="31"/>
       <c r="P89" s="21"/>
-      <c r="S89" s="46"/>
-    </row>
-    <row r="90" spans="7:19">
+      <c r="T89" s="46"/>
+    </row>
+    <row r="90" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G90" s="48"/>
       <c r="H90" s="59"/>
       <c r="J90" s="31"/>
       <c r="P90" s="21"/>
-      <c r="S90" s="46"/>
-    </row>
-    <row r="91" spans="7:19">
+      <c r="T90" s="46"/>
+    </row>
+    <row r="91" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G91" s="48"/>
       <c r="H91" s="59"/>
       <c r="J91" s="31"/>
       <c r="P91" s="21"/>
-      <c r="S91" s="46"/>
-    </row>
-    <row r="92" spans="7:19">
+      <c r="T91" s="46"/>
+    </row>
+    <row r="92" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G92" s="48"/>
       <c r="H92" s="59"/>
       <c r="J92" s="31"/>
       <c r="P92" s="21"/>
-      <c r="S92" s="46"/>
-    </row>
-    <row r="93" spans="7:19">
+      <c r="T92" s="46"/>
+    </row>
+    <row r="93" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G93" s="48"/>
       <c r="H93" s="59"/>
       <c r="J93" s="31"/>
       <c r="P93" s="21"/>
-      <c r="S93" s="46"/>
-    </row>
-    <row r="94" spans="7:19">
+      <c r="T93" s="46"/>
+    </row>
+    <row r="94" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G94" s="48"/>
       <c r="H94" s="59"/>
       <c r="J94" s="31"/>
       <c r="P94" s="21"/>
-      <c r="S94" s="46"/>
-    </row>
-    <row r="95" spans="7:19">
+      <c r="T94" s="46"/>
+    </row>
+    <row r="95" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G95" s="48"/>
       <c r="H95" s="59"/>
       <c r="J95" s="31"/>
       <c r="P95" s="21"/>
-      <c r="S95" s="46"/>
-    </row>
-    <row r="96" spans="7:19">
+      <c r="T95" s="46"/>
+    </row>
+    <row r="96" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G96" s="48"/>
       <c r="H96" s="59"/>
       <c r="J96" s="31"/>
       <c r="P96" s="21"/>
-      <c r="S96" s="46"/>
-    </row>
-    <row r="97" spans="7:19">
+      <c r="T96" s="46"/>
+    </row>
+    <row r="97" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G97" s="48"/>
       <c r="H97" s="59"/>
       <c r="J97" s="31"/>
       <c r="P97" s="21"/>
-      <c r="S97" s="46"/>
-    </row>
-    <row r="98" spans="7:19">
+      <c r="T97" s="46"/>
+    </row>
+    <row r="98" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G98" s="48"/>
       <c r="H98" s="59"/>
       <c r="J98" s="31"/>
       <c r="P98" s="21"/>
-      <c r="S98" s="46"/>
-    </row>
-    <row r="99" spans="7:19">
+      <c r="T98" s="46"/>
+    </row>
+    <row r="99" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G99" s="48"/>
       <c r="H99" s="59"/>
       <c r="J99" s="31"/>
       <c r="P99" s="21"/>
-      <c r="S99" s="46"/>
-    </row>
-    <row r="100" spans="7:19">
+      <c r="T99" s="46"/>
+    </row>
+    <row r="100" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G100" s="48"/>
       <c r="H100" s="59"/>
       <c r="J100" s="31"/>
       <c r="P100" s="21"/>
-      <c r="S100" s="46"/>
-    </row>
-    <row r="101" spans="7:19">
+      <c r="T100" s="46"/>
+    </row>
+    <row r="101" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G101" s="48"/>
       <c r="H101" s="59"/>
       <c r="J101" s="31"/>
       <c r="P101" s="21"/>
-      <c r="S101" s="46"/>
-    </row>
-    <row r="102" spans="7:19">
+      <c r="T101" s="46"/>
+    </row>
+    <row r="102" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G102" s="48"/>
       <c r="H102" s="59"/>
       <c r="J102" s="31"/>
       <c r="P102" s="21"/>
-      <c r="S102" s="46"/>
-    </row>
-    <row r="103" spans="7:19">
+      <c r="T102" s="46"/>
+    </row>
+    <row r="103" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G103" s="48"/>
       <c r="H103" s="59"/>
       <c r="J103" s="31"/>
       <c r="P103" s="21"/>
-      <c r="S103" s="46"/>
-    </row>
-    <row r="104" spans="7:19">
+      <c r="T103" s="46"/>
+    </row>
+    <row r="104" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G104" s="48"/>
       <c r="H104" s="59"/>
       <c r="J104" s="31"/>
       <c r="P104" s="21"/>
-      <c r="S104" s="46"/>
-    </row>
-    <row r="105" spans="7:19">
+      <c r="T104" s="46"/>
+    </row>
+    <row r="105" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G105" s="48"/>
       <c r="H105" s="59"/>
       <c r="J105" s="31"/>
       <c r="P105" s="21"/>
-      <c r="S105" s="46"/>
-    </row>
-    <row r="106" spans="7:19">
+      <c r="T105" s="46"/>
+    </row>
+    <row r="106" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G106" s="48"/>
       <c r="H106" s="59"/>
       <c r="J106" s="31"/>
       <c r="P106" s="21"/>
-      <c r="S106" s="46"/>
-    </row>
-    <row r="107" spans="7:19">
+      <c r="T106" s="46"/>
+    </row>
+    <row r="107" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G107" s="48"/>
       <c r="H107" s="59"/>
       <c r="J107" s="31"/>
       <c r="P107" s="21"/>
-      <c r="S107" s="46"/>
-    </row>
-    <row r="108" spans="7:19">
+      <c r="T107" s="46"/>
+    </row>
+    <row r="108" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G108" s="48"/>
       <c r="H108" s="59"/>
       <c r="J108" s="31"/>
       <c r="P108" s="21"/>
-      <c r="S108" s="46"/>
-    </row>
-    <row r="109" spans="7:19">
+      <c r="T108" s="46"/>
+    </row>
+    <row r="109" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G109" s="48"/>
       <c r="H109" s="59"/>
       <c r="J109" s="31"/>
       <c r="P109" s="21"/>
-      <c r="S109" s="46"/>
-    </row>
-    <row r="110" spans="7:19">
+      <c r="T109" s="46"/>
+    </row>
+    <row r="110" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G110" s="48"/>
       <c r="H110" s="59"/>
       <c r="J110" s="31"/>
       <c r="P110" s="21"/>
-      <c r="S110" s="46"/>
-    </row>
-    <row r="111" spans="7:19">
+      <c r="T110" s="46"/>
+    </row>
+    <row r="111" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G111" s="48"/>
       <c r="H111" s="59"/>
       <c r="J111" s="31"/>
       <c r="P111" s="21"/>
-      <c r="S111" s="46"/>
-    </row>
-    <row r="112" spans="7:19">
+      <c r="T111" s="46"/>
+    </row>
+    <row r="112" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G112" s="48"/>
       <c r="H112" s="59"/>
       <c r="J112" s="31"/>
       <c r="P112" s="21"/>
-      <c r="S112" s="46"/>
-    </row>
-    <row r="113" spans="7:19">
+      <c r="T112" s="46"/>
+    </row>
+    <row r="113" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G113" s="48"/>
       <c r="H113" s="59"/>
       <c r="J113" s="31"/>
       <c r="P113" s="21"/>
-      <c r="S113" s="46"/>
-    </row>
-    <row r="114" spans="7:19">
+      <c r="T113" s="46"/>
+    </row>
+    <row r="114" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G114" s="48"/>
       <c r="H114" s="59"/>
       <c r="J114" s="31"/>
       <c r="P114" s="21"/>
-      <c r="S114" s="46"/>
-    </row>
-    <row r="115" spans="7:19">
+      <c r="T114" s="46"/>
+    </row>
+    <row r="115" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G115" s="48"/>
       <c r="H115" s="59"/>
       <c r="J115" s="31"/>
       <c r="P115" s="21"/>
-      <c r="S115" s="46"/>
-    </row>
-    <row r="116" spans="7:19">
+      <c r="T115" s="46"/>
+    </row>
+    <row r="116" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G116" s="48"/>
       <c r="H116" s="59"/>
       <c r="J116" s="31"/>
       <c r="P116" s="21"/>
-      <c r="S116" s="46"/>
-    </row>
-    <row r="117" spans="7:19">
+      <c r="T116" s="46"/>
+    </row>
+    <row r="117" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G117" s="48"/>
       <c r="H117" s="59"/>
       <c r="J117" s="31"/>
       <c r="P117" s="21"/>
-      <c r="S117" s="46"/>
-    </row>
-    <row r="118" spans="7:19">
+      <c r="T117" s="46"/>
+    </row>
+    <row r="118" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G118" s="48"/>
       <c r="H118" s="59"/>
       <c r="J118" s="31"/>
       <c r="P118" s="21"/>
-      <c r="S118" s="46"/>
-    </row>
-    <row r="119" spans="7:19">
+      <c r="T118" s="46"/>
+    </row>
+    <row r="119" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G119" s="48"/>
       <c r="H119" s="59"/>
       <c r="J119" s="31"/>
       <c r="P119" s="21"/>
-      <c r="S119" s="46"/>
-    </row>
-    <row r="120" spans="7:19">
+      <c r="T119" s="46"/>
+    </row>
+    <row r="120" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G120" s="48"/>
       <c r="H120" s="59"/>
       <c r="J120" s="31"/>
       <c r="P120" s="21"/>
-      <c r="S120" s="46"/>
-    </row>
-    <row r="121" spans="7:19">
+      <c r="T120" s="46"/>
+    </row>
+    <row r="121" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G121" s="48"/>
       <c r="H121" s="59"/>
       <c r="J121" s="31"/>
       <c r="P121" s="21"/>
-      <c r="S121" s="46"/>
-    </row>
-    <row r="122" spans="7:19">
+      <c r="T121" s="46"/>
+    </row>
+    <row r="122" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G122" s="48"/>
       <c r="H122" s="59"/>
       <c r="J122" s="31"/>
       <c r="P122" s="21"/>
-      <c r="S122" s="46"/>
-    </row>
-    <row r="123" spans="7:19">
+      <c r="T122" s="46"/>
+    </row>
+    <row r="123" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G123" s="48"/>
       <c r="H123" s="59"/>
       <c r="J123" s="31"/>
       <c r="P123" s="21"/>
-      <c r="S123" s="46"/>
-    </row>
-    <row r="124" spans="7:19">
+      <c r="T123" s="46"/>
+    </row>
+    <row r="124" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G124" s="48"/>
       <c r="H124" s="59"/>
       <c r="J124" s="31"/>
       <c r="P124" s="21"/>
-      <c r="S124" s="46"/>
-    </row>
-    <row r="125" spans="7:19">
+      <c r="T124" s="46"/>
+    </row>
+    <row r="125" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G125" s="48"/>
       <c r="H125" s="59"/>
       <c r="J125" s="31"/>
       <c r="P125" s="21"/>
-      <c r="S125" s="46"/>
-    </row>
-    <row r="126" spans="7:19">
+      <c r="T125" s="46"/>
+    </row>
+    <row r="126" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G126" s="48"/>
       <c r="H126" s="59"/>
       <c r="J126" s="31"/>
       <c r="P126" s="21"/>
-      <c r="S126" s="46"/>
-    </row>
-    <row r="127" spans="7:19">
+      <c r="T126" s="46"/>
+    </row>
+    <row r="127" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G127" s="48"/>
       <c r="H127" s="59"/>
       <c r="J127" s="31"/>
       <c r="P127" s="21"/>
-      <c r="S127" s="46"/>
-    </row>
-    <row r="128" spans="7:19">
+      <c r="T127" s="46"/>
+    </row>
+    <row r="128" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G128" s="48"/>
       <c r="H128" s="59"/>
       <c r="J128" s="31"/>
       <c r="P128" s="21"/>
-      <c r="S128" s="46"/>
-    </row>
-    <row r="129" spans="7:19">
+      <c r="T128" s="46"/>
+    </row>
+    <row r="129" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G129" s="48"/>
       <c r="H129" s="59"/>
       <c r="J129" s="31"/>
       <c r="P129" s="21"/>
-      <c r="S129" s="46"/>
-    </row>
-    <row r="130" spans="7:19">
+      <c r="T129" s="46"/>
+    </row>
+    <row r="130" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G130" s="48"/>
       <c r="H130" s="59"/>
       <c r="J130" s="31"/>
       <c r="P130" s="21"/>
-      <c r="S130" s="46"/>
-    </row>
-    <row r="131" spans="7:19">
+      <c r="T130" s="46"/>
+    </row>
+    <row r="131" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G131" s="48"/>
       <c r="H131" s="59"/>
       <c r="J131" s="31"/>
       <c r="P131" s="21"/>
-      <c r="S131" s="46"/>
-    </row>
-    <row r="132" spans="7:19">
+      <c r="T131" s="46"/>
+    </row>
+    <row r="132" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G132" s="48"/>
       <c r="H132" s="59"/>
       <c r="J132" s="31"/>
       <c r="P132" s="21"/>
-      <c r="S132" s="46"/>
-    </row>
-    <row r="133" spans="7:19">
+      <c r="T132" s="46"/>
+    </row>
+    <row r="133" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G133" s="48"/>
       <c r="H133" s="59"/>
       <c r="J133" s="31"/>
       <c r="P133" s="21"/>
-      <c r="S133" s="46"/>
-    </row>
-    <row r="134" spans="7:19">
+      <c r="T133" s="46"/>
+    </row>
+    <row r="134" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G134" s="48"/>
       <c r="H134" s="59"/>
       <c r="J134" s="31"/>
       <c r="P134" s="21"/>
-      <c r="S134" s="46"/>
-    </row>
-    <row r="135" spans="7:19">
+      <c r="T134" s="46"/>
+    </row>
+    <row r="135" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G135" s="48"/>
       <c r="H135" s="59"/>
       <c r="J135" s="31"/>
       <c r="P135" s="21"/>
-      <c r="S135" s="46"/>
-    </row>
-    <row r="136" spans="7:19">
+      <c r="T135" s="46"/>
+    </row>
+    <row r="136" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G136" s="48"/>
       <c r="H136" s="59"/>
       <c r="J136" s="31"/>
       <c r="P136" s="21"/>
-      <c r="S136" s="46"/>
-    </row>
-    <row r="137" spans="7:19">
+      <c r="T136" s="46"/>
+    </row>
+    <row r="137" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G137" s="48"/>
       <c r="H137" s="59"/>
       <c r="J137" s="31"/>
       <c r="P137" s="21"/>
-      <c r="S137" s="46"/>
-    </row>
-    <row r="138" spans="7:19">
+      <c r="T137" s="46"/>
+    </row>
+    <row r="138" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G138" s="48"/>
       <c r="H138" s="59"/>
       <c r="J138" s="31"/>
       <c r="P138" s="21"/>
-      <c r="S138" s="46"/>
-    </row>
-    <row r="139" spans="7:19">
+      <c r="T138" s="46"/>
+    </row>
+    <row r="139" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G139" s="48"/>
       <c r="H139" s="59"/>
       <c r="J139" s="31"/>
       <c r="P139" s="21"/>
-      <c r="S139" s="46"/>
-    </row>
-    <row r="140" spans="7:19">
+      <c r="T139" s="46"/>
+    </row>
+    <row r="140" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G140" s="48"/>
       <c r="H140" s="59"/>
       <c r="J140" s="31"/>
       <c r="P140" s="21"/>
-      <c r="S140" s="46"/>
-    </row>
-    <row r="141" spans="7:19">
+      <c r="T140" s="46"/>
+    </row>
+    <row r="141" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G141" s="48"/>
       <c r="H141" s="59"/>
       <c r="J141" s="31"/>
       <c r="P141" s="21"/>
-      <c r="S141" s="46"/>
-    </row>
-    <row r="142" spans="7:19">
+      <c r="T141" s="46"/>
+    </row>
+    <row r="142" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G142" s="48"/>
       <c r="H142" s="59"/>
       <c r="J142" s="31"/>
       <c r="P142" s="21"/>
-      <c r="S142" s="46"/>
-    </row>
-    <row r="143" spans="7:19">
+      <c r="T142" s="46"/>
+    </row>
+    <row r="143" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G143" s="48"/>
       <c r="H143" s="59"/>
       <c r="J143" s="31"/>
       <c r="P143" s="21"/>
-      <c r="S143" s="46"/>
-    </row>
-    <row r="144" spans="7:19">
+      <c r="T143" s="46"/>
+    </row>
+    <row r="144" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G144" s="48"/>
       <c r="H144" s="59"/>
       <c r="J144" s="31"/>
       <c r="P144" s="21"/>
-      <c r="S144" s="46"/>
-    </row>
-    <row r="145" spans="7:19">
+      <c r="T144" s="46"/>
+    </row>
+    <row r="145" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G145" s="48"/>
       <c r="H145" s="59"/>
       <c r="J145" s="31"/>
       <c r="P145" s="21"/>
-      <c r="S145" s="46"/>
-    </row>
-    <row r="146" spans="7:19">
+      <c r="T145" s="46"/>
+    </row>
+    <row r="146" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G146" s="48"/>
       <c r="H146" s="59"/>
       <c r="J146" s="31"/>
       <c r="P146" s="21"/>
-      <c r="S146" s="46"/>
-    </row>
-    <row r="147" spans="7:19">
+      <c r="T146" s="46"/>
+    </row>
+    <row r="147" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G147" s="48"/>
       <c r="H147" s="59"/>
       <c r="J147" s="31"/>
       <c r="P147" s="21"/>
-      <c r="S147" s="46"/>
-    </row>
-    <row r="148" spans="7:19">
+      <c r="T147" s="46"/>
+    </row>
+    <row r="148" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G148" s="48"/>
       <c r="H148" s="59"/>
       <c r="J148" s="31"/>
       <c r="P148" s="21"/>
-      <c r="S148" s="46"/>
-    </row>
-    <row r="149" spans="7:19">
+      <c r="T148" s="46"/>
+    </row>
+    <row r="149" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G149" s="48"/>
       <c r="H149" s="59"/>
       <c r="J149" s="31"/>
       <c r="P149" s="21"/>
-      <c r="S149" s="46"/>
-    </row>
-    <row r="150" spans="7:19">
+      <c r="T149" s="46"/>
+    </row>
+    <row r="150" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G150" s="48"/>
       <c r="H150" s="59"/>
       <c r="J150" s="31"/>
       <c r="P150" s="21"/>
-      <c r="S150" s="46"/>
-    </row>
-    <row r="151" spans="7:19">
+      <c r="T150" s="46"/>
+    </row>
+    <row r="151" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G151" s="48"/>
       <c r="H151" s="59"/>
       <c r="J151" s="31"/>
       <c r="P151" s="21"/>
-      <c r="S151" s="46"/>
-    </row>
-    <row r="152" spans="7:19">
+      <c r="T151" s="46"/>
+    </row>
+    <row r="152" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G152" s="48"/>
       <c r="H152" s="59"/>
       <c r="J152" s="31"/>
       <c r="P152" s="21"/>
-      <c r="S152" s="46"/>
-    </row>
-    <row r="153" spans="7:19">
+      <c r="T152" s="46"/>
+    </row>
+    <row r="153" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G153" s="48"/>
       <c r="H153" s="59"/>
       <c r="J153" s="31"/>
       <c r="P153" s="21"/>
-      <c r="S153" s="46"/>
-    </row>
-    <row r="154" spans="7:19">
+      <c r="T153" s="46"/>
+    </row>
+    <row r="154" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G154" s="48"/>
       <c r="H154" s="60"/>
     </row>
-    <row r="155" spans="7:19">
+    <row r="155" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G155" s="48"/>
       <c r="H155" s="60"/>
     </row>
-    <row r="156" spans="7:19">
+    <row r="156" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G156" s="48"/>
       <c r="H156" s="60"/>
     </row>
-    <row r="157" spans="7:19">
+    <row r="157" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G157" s="48"/>
       <c r="H157" s="60"/>
     </row>
-    <row r="158" spans="7:19">
+    <row r="158" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G158" s="48"/>
       <c r="H158" s="60"/>
     </row>
-    <row r="159" spans="7:19">
+    <row r="159" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G159" s="48"/>
       <c r="H159" s="60"/>
     </row>
-    <row r="160" spans="7:19">
+    <row r="160" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G160" s="48"/>
       <c r="H160" s="60"/>
     </row>
-    <row r="161" spans="7:8">
+    <row r="161" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G161" s="48"/>
       <c r="H161" s="60"/>
     </row>
-    <row r="162" spans="7:8">
+    <row r="162" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G162" s="48"/>
       <c r="H162" s="60"/>
     </row>
-    <row r="163" spans="7:8">
+    <row r="163" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G163" s="48"/>
       <c r="H163" s="60"/>
     </row>
-    <row r="164" spans="7:8">
+    <row r="164" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G164" s="48"/>
       <c r="H164" s="60"/>
     </row>
-    <row r="165" spans="7:8">
+    <row r="165" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G165" s="48"/>
       <c r="H165" s="60"/>
     </row>
-    <row r="166" spans="7:8">
+    <row r="166" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G166" s="48"/>
       <c r="H166" s="60"/>
     </row>
-    <row r="167" spans="7:8">
+    <row r="167" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G167" s="48"/>
       <c r="H167" s="60"/>
     </row>
-    <row r="168" spans="7:8">
+    <row r="168" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G168" s="48"/>
       <c r="H168" s="60"/>
     </row>
-    <row r="169" spans="7:8">
+    <row r="169" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G169" s="48"/>
       <c r="H169" s="60"/>
     </row>
-    <row r="170" spans="7:8">
+    <row r="170" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G170" s="48"/>
       <c r="H170" s="60"/>
     </row>
-    <row r="171" spans="7:8">
+    <row r="171" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G171" s="48"/>
       <c r="H171" s="60"/>
     </row>
-    <row r="172" spans="7:8">
+    <row r="172" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G172" s="48"/>
       <c r="H172" s="60"/>
     </row>
-    <row r="173" spans="7:8">
+    <row r="173" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G173" s="48"/>
       <c r="H173" s="60"/>
     </row>
-    <row r="174" spans="7:8">
+    <row r="174" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G174" s="48"/>
       <c r="H174" s="60"/>
     </row>
-    <row r="175" spans="7:8">
+    <row r="175" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G175" s="48"/>
       <c r="H175" s="60"/>
     </row>
-    <row r="176" spans="7:8">
+    <row r="176" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G176" s="48"/>
       <c r="H176" s="60"/>
     </row>
-    <row r="177" spans="7:8">
+    <row r="177" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G177" s="48"/>
       <c r="H177" s="60"/>
     </row>
-    <row r="178" spans="7:8">
+    <row r="178" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G178" s="48"/>
       <c r="H178" s="60"/>
     </row>
-    <row r="179" spans="7:8">
+    <row r="179" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G179" s="48"/>
       <c r="H179" s="60"/>
     </row>
-    <row r="180" spans="7:8">
+    <row r="180" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G180" s="48"/>
       <c r="H180" s="60"/>
     </row>
-    <row r="181" spans="7:8">
+    <row r="181" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G181" s="48"/>
       <c r="H181" s="60"/>
     </row>
-    <row r="182" spans="7:8">
+    <row r="182" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G182" s="48"/>
       <c r="H182" s="60"/>
     </row>
-    <row r="183" spans="7:8">
+    <row r="183" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G183" s="48"/>
       <c r="H183" s="60"/>
     </row>
-    <row r="184" spans="7:8">
+    <row r="184" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G184" s="48"/>
       <c r="H184" s="60"/>
     </row>
-    <row r="185" spans="7:8">
+    <row r="185" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G185" s="48"/>
       <c r="H185" s="60"/>
     </row>
-    <row r="186" spans="7:8">
+    <row r="186" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G186" s="48"/>
       <c r="H186" s="60"/>
     </row>
-    <row r="187" spans="7:8">
+    <row r="187" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G187" s="48"/>
       <c r="H187" s="60"/>
     </row>
-    <row r="188" spans="7:8">
+    <row r="188" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G188" s="48"/>
       <c r="H188" s="60"/>
     </row>
-    <row r="189" spans="7:8">
+    <row r="189" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G189" s="48"/>
       <c r="H189" s="60"/>
     </row>
-    <row r="190" spans="7:8">
+    <row r="190" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G190" s="48"/>
       <c r="H190" s="60"/>
     </row>
-    <row r="191" spans="7:8">
+    <row r="191" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G191" s="48"/>
       <c r="H191" s="60"/>
     </row>
-    <row r="192" spans="7:8">
+    <row r="192" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G192" s="48"/>
       <c r="H192" s="60"/>
     </row>
-    <row r="193" spans="7:8">
+    <row r="193" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G193" s="48"/>
       <c r="H193" s="60"/>
     </row>
-    <row r="194" spans="7:8">
+    <row r="194" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G194" s="48"/>
       <c r="H194" s="60"/>
     </row>
-    <row r="195" spans="7:8">
+    <row r="195" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G195" s="48"/>
       <c r="H195" s="60"/>
     </row>
-    <row r="196" spans="7:8">
+    <row r="196" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G196" s="48"/>
       <c r="H196" s="60"/>
     </row>
-    <row r="197" spans="7:8">
+    <row r="197" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G197" s="48"/>
       <c r="H197" s="60"/>
     </row>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="A1:I1"/>
-    <mergeCell ref="K1:R1"/>
-    <mergeCell ref="T1:Z1"/>
+    <mergeCell ref="K1:S1"/>
+    <mergeCell ref="U1:AA1"/>
+    <mergeCell ref="A2:I2"/>
     <mergeCell ref="K2:M2"/>
-    <mergeCell ref="R2:R3"/>
-    <mergeCell ref="A2:I2"/>
     <mergeCell ref="N2:P2"/>
+    <mergeCell ref="S2:S3"/>
   </mergeCells>
+  <phoneticPr fontId="37" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter>
@@ -3761,23 +3738,1776 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AA197"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:I1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8" customWidth="1"/>
+    <col min="2" max="2" width="6.42578125" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+    <col min="7" max="7" width="4.140625" style="28" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" style="61" customWidth="1"/>
+    <col min="9" max="9" width="8.85546875" customWidth="1"/>
+    <col min="10" max="10" width="4.7109375" customWidth="1"/>
+    <col min="11" max="11" width="14" customWidth="1"/>
+    <col min="12" max="12" width="8.7109375" style="28" customWidth="1"/>
+    <col min="13" max="13" width="10.85546875" style="28" customWidth="1"/>
+    <col min="14" max="14" width="14" customWidth="1"/>
+    <col min="15" max="15" width="7.5703125" customWidth="1"/>
+    <col min="16" max="16" width="13.140625" customWidth="1"/>
+    <col min="17" max="17" width="22.42578125" customWidth="1"/>
+    <col min="18" max="18" width="10.42578125" style="28" customWidth="1"/>
+    <col min="20" max="20" width="4.7109375" customWidth="1"/>
+    <col min="21" max="21" width="12.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.42578125" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="31.28515625" style="48" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="8.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" s="4" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="64" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
+      <c r="I1" s="64"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="65" t="s">
+        <v>54</v>
+      </c>
+      <c r="L1" s="65"/>
+      <c r="M1" s="65"/>
+      <c r="N1" s="65"/>
+      <c r="O1" s="65"/>
+      <c r="P1" s="65"/>
+      <c r="Q1" s="66"/>
+      <c r="R1" s="75"/>
+      <c r="S1" s="67"/>
+      <c r="T1" s="42"/>
+      <c r="U1" s="68" t="s">
+        <v>11</v>
+      </c>
+      <c r="V1" s="65"/>
+      <c r="W1" s="65"/>
+      <c r="X1" s="65"/>
+      <c r="Y1" s="65"/>
+      <c r="Z1" s="65"/>
+      <c r="AA1" s="65"/>
+    </row>
+    <row r="2" spans="1:27" s="4" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="74"/>
+      <c r="B2" s="74"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="69" t="s">
+        <v>61</v>
+      </c>
+      <c r="L2" s="70"/>
+      <c r="M2" s="71"/>
+      <c r="N2" s="69" t="s">
+        <v>55</v>
+      </c>
+      <c r="O2" s="70"/>
+      <c r="P2" s="70"/>
+      <c r="Q2" s="51"/>
+      <c r="R2" s="51"/>
+      <c r="S2" s="72" t="s">
+        <v>75</v>
+      </c>
+      <c r="T2" s="42"/>
+      <c r="U2" s="55"/>
+      <c r="V2" s="56"/>
+      <c r="W2" s="53" t="s">
+        <v>74</v>
+      </c>
+      <c r="X2" s="58"/>
+      <c r="Y2" s="58"/>
+      <c r="Z2" s="54"/>
+      <c r="AA2" s="57"/>
+    </row>
+    <row r="3" spans="1:27" s="7" customFormat="1" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J3" s="6"/>
+      <c r="K3" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="L3" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="M3" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="N3" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="O3" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="P3" s="50" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q3" s="52" t="s">
+        <v>68</v>
+      </c>
+      <c r="R3" s="76" t="s">
+        <v>78</v>
+      </c>
+      <c r="S3" s="73"/>
+      <c r="T3" s="43"/>
+      <c r="U3" s="41" t="s">
+        <v>6</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z3" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA3" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D4" s="19"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="59"/>
+      <c r="J4" s="20"/>
+      <c r="L4" s="29"/>
+      <c r="M4" s="29"/>
+      <c r="P4" s="21"/>
+      <c r="R4" s="29"/>
+      <c r="T4" s="44"/>
+      <c r="U4" s="21"/>
+      <c r="Z4" s="49"/>
+    </row>
+    <row r="5" spans="1:27" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D5" s="19"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="59"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="29"/>
+      <c r="L5" s="29"/>
+      <c r="M5" s="29"/>
+      <c r="P5" s="21"/>
+      <c r="R5" s="29"/>
+      <c r="T5" s="45"/>
+      <c r="U5" s="21"/>
+      <c r="Z5" s="49"/>
+    </row>
+    <row r="6" spans="1:27" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D6" s="19"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="59"/>
+      <c r="I6" s="27"/>
+      <c r="J6" s="20"/>
+      <c r="L6" s="29"/>
+      <c r="M6" s="29"/>
+      <c r="P6" s="21"/>
+      <c r="R6" s="29"/>
+      <c r="T6" s="45"/>
+      <c r="U6" s="21"/>
+      <c r="Z6" s="49"/>
+    </row>
+    <row r="7" spans="1:27" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D7" s="19"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="59"/>
+      <c r="J7" s="20"/>
+      <c r="L7" s="29"/>
+      <c r="M7" s="29"/>
+      <c r="P7" s="21"/>
+      <c r="R7" s="29"/>
+      <c r="T7" s="45"/>
+      <c r="U7" s="21"/>
+      <c r="Z7" s="49"/>
+    </row>
+    <row r="8" spans="1:27" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D8" s="19"/>
+      <c r="G8" s="47"/>
+      <c r="H8" s="59"/>
+      <c r="J8" s="20"/>
+      <c r="L8" s="29"/>
+      <c r="M8" s="29"/>
+      <c r="P8" s="21"/>
+      <c r="R8" s="29"/>
+      <c r="T8" s="45"/>
+      <c r="U8" s="21"/>
+      <c r="Z8" s="49"/>
+    </row>
+    <row r="9" spans="1:27" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D9" s="19"/>
+      <c r="G9" s="47"/>
+      <c r="H9" s="59"/>
+      <c r="J9" s="20"/>
+      <c r="L9" s="29"/>
+      <c r="M9" s="29"/>
+      <c r="P9" s="21"/>
+      <c r="R9" s="29"/>
+      <c r="T9" s="45"/>
+      <c r="U9" s="21"/>
+      <c r="Z9" s="47"/>
+    </row>
+    <row r="10" spans="1:27" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D10" s="19"/>
+      <c r="G10" s="47"/>
+      <c r="H10" s="59"/>
+      <c r="J10" s="20"/>
+      <c r="L10" s="29"/>
+      <c r="M10" s="29"/>
+      <c r="P10" s="21"/>
+      <c r="R10" s="29"/>
+      <c r="T10" s="45"/>
+      <c r="U10" s="21"/>
+      <c r="Z10" s="47"/>
+    </row>
+    <row r="11" spans="1:27" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D11" s="19"/>
+      <c r="G11" s="47"/>
+      <c r="H11" s="59"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="20"/>
+      <c r="L11" s="29"/>
+      <c r="M11" s="29"/>
+      <c r="P11" s="21"/>
+      <c r="R11" s="29"/>
+      <c r="T11" s="45"/>
+      <c r="U11" s="21"/>
+      <c r="Z11" s="47"/>
+    </row>
+    <row r="12" spans="1:27" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D12" s="19"/>
+      <c r="G12" s="47"/>
+      <c r="H12" s="59"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="20"/>
+      <c r="L12" s="29"/>
+      <c r="M12" s="29"/>
+      <c r="P12" s="21"/>
+      <c r="R12" s="29"/>
+      <c r="T12" s="45"/>
+      <c r="U12" s="21"/>
+      <c r="Z12" s="49"/>
+    </row>
+    <row r="13" spans="1:27" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D13" s="19"/>
+      <c r="G13" s="47"/>
+      <c r="H13" s="59"/>
+      <c r="J13" s="20"/>
+      <c r="L13" s="29"/>
+      <c r="M13" s="29"/>
+      <c r="P13" s="21"/>
+      <c r="R13" s="29"/>
+      <c r="T13" s="45"/>
+      <c r="U13" s="21"/>
+      <c r="Z13" s="47"/>
+    </row>
+    <row r="14" spans="1:27" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D14" s="19"/>
+      <c r="G14" s="47"/>
+      <c r="H14" s="59"/>
+      <c r="J14" s="20"/>
+      <c r="L14" s="29"/>
+      <c r="M14" s="29"/>
+      <c r="P14" s="21"/>
+      <c r="R14" s="29"/>
+      <c r="T14" s="45"/>
+      <c r="U14" s="21"/>
+      <c r="Z14" s="47"/>
+    </row>
+    <row r="15" spans="1:27" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D15" s="19"/>
+      <c r="G15" s="47"/>
+      <c r="H15" s="59"/>
+      <c r="J15" s="20"/>
+      <c r="L15" s="29"/>
+      <c r="M15" s="29"/>
+      <c r="P15" s="21"/>
+      <c r="R15" s="29"/>
+      <c r="T15" s="45"/>
+      <c r="U15" s="21"/>
+      <c r="Z15" s="47"/>
+    </row>
+    <row r="16" spans="1:27" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D16" s="19"/>
+      <c r="G16" s="47"/>
+      <c r="H16" s="59"/>
+      <c r="J16" s="20"/>
+      <c r="L16" s="29"/>
+      <c r="M16" s="29"/>
+      <c r="P16" s="21"/>
+      <c r="R16" s="29"/>
+      <c r="T16" s="45"/>
+      <c r="U16" s="21"/>
+      <c r="Z16" s="47"/>
+    </row>
+    <row r="17" spans="4:26" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D17" s="19"/>
+      <c r="G17" s="47"/>
+      <c r="H17" s="59"/>
+      <c r="J17" s="20"/>
+      <c r="L17" s="29"/>
+      <c r="M17" s="29"/>
+      <c r="P17" s="21"/>
+      <c r="R17" s="29"/>
+      <c r="T17" s="45"/>
+      <c r="U17" s="21"/>
+      <c r="Z17" s="47"/>
+    </row>
+    <row r="18" spans="4:26" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D18" s="19"/>
+      <c r="G18" s="47"/>
+      <c r="H18" s="59"/>
+      <c r="J18" s="20"/>
+      <c r="L18" s="29"/>
+      <c r="M18" s="29"/>
+      <c r="P18" s="21"/>
+      <c r="R18" s="29"/>
+      <c r="T18" s="45"/>
+      <c r="U18" s="21"/>
+      <c r="Z18" s="47"/>
+    </row>
+    <row r="19" spans="4:26" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D19" s="19"/>
+      <c r="G19" s="47"/>
+      <c r="H19" s="59"/>
+      <c r="J19" s="20"/>
+      <c r="L19" s="29"/>
+      <c r="M19" s="29"/>
+      <c r="P19" s="21"/>
+      <c r="R19" s="29"/>
+      <c r="T19" s="45"/>
+      <c r="U19" s="21"/>
+      <c r="Z19" s="47"/>
+    </row>
+    <row r="20" spans="4:26" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D20" s="19"/>
+      <c r="G20" s="47"/>
+      <c r="H20" s="59"/>
+      <c r="J20" s="20"/>
+      <c r="L20" s="29"/>
+      <c r="M20" s="29"/>
+      <c r="P20" s="21"/>
+      <c r="R20" s="29"/>
+      <c r="T20" s="45"/>
+      <c r="U20" s="21"/>
+      <c r="Z20" s="47"/>
+    </row>
+    <row r="21" spans="4:26" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D21" s="19"/>
+      <c r="G21" s="47"/>
+      <c r="H21" s="59"/>
+      <c r="J21" s="20"/>
+      <c r="L21" s="29"/>
+      <c r="M21" s="29"/>
+      <c r="P21" s="21"/>
+      <c r="R21" s="29"/>
+      <c r="T21" s="45"/>
+      <c r="U21" s="21"/>
+      <c r="Z21" s="47"/>
+    </row>
+    <row r="22" spans="4:26" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D22" s="19"/>
+      <c r="G22" s="47"/>
+      <c r="H22" s="59"/>
+      <c r="J22" s="20"/>
+      <c r="L22" s="29"/>
+      <c r="M22" s="29"/>
+      <c r="P22" s="21"/>
+      <c r="R22" s="29"/>
+      <c r="T22" s="45"/>
+      <c r="U22" s="21"/>
+      <c r="Z22" s="47"/>
+    </row>
+    <row r="23" spans="4:26" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D23" s="19"/>
+      <c r="G23" s="47"/>
+      <c r="H23" s="59"/>
+      <c r="J23" s="20"/>
+      <c r="L23" s="29"/>
+      <c r="M23" s="29"/>
+      <c r="P23" s="21"/>
+      <c r="R23" s="29"/>
+      <c r="T23" s="45"/>
+      <c r="U23" s="21"/>
+      <c r="Z23" s="47"/>
+    </row>
+    <row r="24" spans="4:26" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D24" s="19"/>
+      <c r="G24" s="47"/>
+      <c r="H24" s="59"/>
+      <c r="J24" s="20"/>
+      <c r="L24" s="29"/>
+      <c r="M24" s="29"/>
+      <c r="P24" s="21"/>
+      <c r="R24" s="29"/>
+      <c r="T24" s="45"/>
+      <c r="U24" s="21"/>
+      <c r="Z24" s="47"/>
+    </row>
+    <row r="25" spans="4:26" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D25" s="19"/>
+      <c r="G25" s="47"/>
+      <c r="H25" s="59"/>
+      <c r="J25" s="20"/>
+      <c r="L25" s="29"/>
+      <c r="M25" s="29"/>
+      <c r="P25" s="21"/>
+      <c r="R25" s="29"/>
+      <c r="T25" s="45"/>
+      <c r="U25" s="21"/>
+      <c r="Z25" s="47"/>
+    </row>
+    <row r="26" spans="4:26" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D26" s="19"/>
+      <c r="G26" s="47"/>
+      <c r="H26" s="59"/>
+      <c r="J26" s="20"/>
+      <c r="L26" s="29"/>
+      <c r="M26" s="29"/>
+      <c r="P26" s="21"/>
+      <c r="R26" s="29"/>
+      <c r="T26" s="45"/>
+      <c r="U26" s="21"/>
+      <c r="Z26" s="47"/>
+    </row>
+    <row r="27" spans="4:26" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D27" s="19"/>
+      <c r="G27" s="47"/>
+      <c r="H27" s="59"/>
+      <c r="J27" s="20"/>
+      <c r="L27" s="29"/>
+      <c r="M27" s="29"/>
+      <c r="P27" s="21"/>
+      <c r="R27" s="29"/>
+      <c r="T27" s="45"/>
+      <c r="U27" s="21"/>
+      <c r="Z27" s="47"/>
+    </row>
+    <row r="28" spans="4:26" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D28" s="19"/>
+      <c r="G28" s="47"/>
+      <c r="H28" s="59"/>
+      <c r="J28" s="20"/>
+      <c r="L28" s="29"/>
+      <c r="M28" s="29"/>
+      <c r="P28" s="21"/>
+      <c r="R28" s="29"/>
+      <c r="T28" s="45"/>
+      <c r="U28" s="21"/>
+      <c r="Z28" s="47"/>
+    </row>
+    <row r="29" spans="4:26" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D29" s="19"/>
+      <c r="G29" s="47"/>
+      <c r="H29" s="59"/>
+      <c r="J29" s="20"/>
+      <c r="L29" s="29"/>
+      <c r="M29" s="29"/>
+      <c r="P29" s="21"/>
+      <c r="R29" s="29"/>
+      <c r="T29" s="45"/>
+      <c r="U29" s="21"/>
+      <c r="Z29" s="47"/>
+    </row>
+    <row r="30" spans="4:26" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D30" s="19"/>
+      <c r="G30" s="47"/>
+      <c r="H30" s="59"/>
+      <c r="J30" s="20"/>
+      <c r="L30" s="29"/>
+      <c r="M30" s="29"/>
+      <c r="P30" s="21"/>
+      <c r="R30" s="29"/>
+      <c r="T30" s="45"/>
+      <c r="U30" s="21"/>
+      <c r="Z30" s="47"/>
+    </row>
+    <row r="31" spans="4:26" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D31" s="19"/>
+      <c r="G31" s="47"/>
+      <c r="H31" s="59"/>
+      <c r="J31" s="20"/>
+      <c r="L31" s="29"/>
+      <c r="M31" s="29"/>
+      <c r="P31" s="21"/>
+      <c r="R31" s="29"/>
+      <c r="T31" s="45"/>
+      <c r="U31" s="21"/>
+      <c r="Z31" s="47"/>
+    </row>
+    <row r="32" spans="4:26" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D32" s="19"/>
+      <c r="G32" s="47"/>
+      <c r="H32" s="59"/>
+      <c r="J32" s="20"/>
+      <c r="L32" s="29"/>
+      <c r="M32" s="29"/>
+      <c r="P32" s="21"/>
+      <c r="R32" s="29"/>
+      <c r="T32" s="45"/>
+      <c r="U32" s="21"/>
+      <c r="Z32" s="47"/>
+    </row>
+    <row r="33" spans="4:26" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D33" s="19"/>
+      <c r="G33" s="47"/>
+      <c r="H33" s="59"/>
+      <c r="J33" s="20"/>
+      <c r="L33" s="29"/>
+      <c r="M33" s="29"/>
+      <c r="P33" s="21"/>
+      <c r="R33" s="29"/>
+      <c r="T33" s="45"/>
+      <c r="U33" s="21"/>
+      <c r="Z33" s="47"/>
+    </row>
+    <row r="34" spans="4:26" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D34" s="19"/>
+      <c r="G34" s="47"/>
+      <c r="H34" s="59"/>
+      <c r="J34" s="20"/>
+      <c r="L34" s="29"/>
+      <c r="M34" s="29"/>
+      <c r="P34" s="21"/>
+      <c r="R34" s="29"/>
+      <c r="T34" s="45"/>
+      <c r="U34" s="21"/>
+      <c r="Z34" s="47"/>
+    </row>
+    <row r="35" spans="4:26" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D35" s="19"/>
+      <c r="G35" s="47"/>
+      <c r="H35" s="59"/>
+      <c r="J35" s="20"/>
+      <c r="L35" s="29"/>
+      <c r="M35" s="29"/>
+      <c r="P35" s="21"/>
+      <c r="R35" s="29"/>
+      <c r="T35" s="45"/>
+      <c r="U35" s="21"/>
+      <c r="Z35" s="47"/>
+    </row>
+    <row r="36" spans="4:26" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D36" s="19"/>
+      <c r="G36" s="47"/>
+      <c r="H36" s="59"/>
+      <c r="J36" s="20"/>
+      <c r="L36" s="29"/>
+      <c r="M36" s="29"/>
+      <c r="P36" s="21"/>
+      <c r="R36" s="29"/>
+      <c r="T36" s="45"/>
+      <c r="U36" s="21"/>
+      <c r="Z36" s="47"/>
+    </row>
+    <row r="37" spans="4:26" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D37" s="19"/>
+      <c r="G37" s="47"/>
+      <c r="H37" s="59"/>
+      <c r="J37" s="20"/>
+      <c r="L37" s="29"/>
+      <c r="M37" s="29"/>
+      <c r="P37" s="21"/>
+      <c r="R37" s="29"/>
+      <c r="T37" s="45"/>
+      <c r="U37" s="21"/>
+      <c r="Z37" s="47"/>
+    </row>
+    <row r="38" spans="4:26" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D38" s="19"/>
+      <c r="G38" s="47"/>
+      <c r="H38" s="59"/>
+      <c r="J38" s="20"/>
+      <c r="L38" s="29"/>
+      <c r="M38" s="29"/>
+      <c r="P38" s="21"/>
+      <c r="R38" s="29"/>
+      <c r="T38" s="45"/>
+      <c r="U38" s="21"/>
+      <c r="Z38" s="47"/>
+    </row>
+    <row r="39" spans="4:26" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D39" s="19"/>
+      <c r="G39" s="47"/>
+      <c r="H39" s="59"/>
+      <c r="J39" s="20"/>
+      <c r="L39" s="29"/>
+      <c r="M39" s="29"/>
+      <c r="P39" s="21"/>
+      <c r="R39" s="29"/>
+      <c r="T39" s="45"/>
+      <c r="U39" s="21"/>
+      <c r="Z39" s="47"/>
+    </row>
+    <row r="40" spans="4:26" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D40" s="19"/>
+      <c r="G40" s="47"/>
+      <c r="H40" s="59"/>
+      <c r="J40" s="20"/>
+      <c r="L40" s="29"/>
+      <c r="M40" s="29"/>
+      <c r="P40" s="21"/>
+      <c r="R40" s="29"/>
+      <c r="T40" s="45"/>
+      <c r="U40" s="21"/>
+      <c r="Z40" s="47"/>
+    </row>
+    <row r="41" spans="4:26" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D41" s="19"/>
+      <c r="G41" s="47"/>
+      <c r="H41" s="59"/>
+      <c r="J41" s="20"/>
+      <c r="L41" s="29"/>
+      <c r="M41" s="29"/>
+      <c r="P41" s="21"/>
+      <c r="R41" s="29"/>
+      <c r="T41" s="45"/>
+      <c r="U41" s="21"/>
+      <c r="Z41" s="47"/>
+    </row>
+    <row r="42" spans="4:26" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D42" s="19"/>
+      <c r="G42" s="47"/>
+      <c r="H42" s="59"/>
+      <c r="J42" s="20"/>
+      <c r="L42" s="29"/>
+      <c r="M42" s="29"/>
+      <c r="P42" s="21"/>
+      <c r="R42" s="29"/>
+      <c r="T42" s="45"/>
+      <c r="U42" s="21"/>
+      <c r="Z42" s="47"/>
+    </row>
+    <row r="43" spans="4:26" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D43" s="19"/>
+      <c r="G43" s="47"/>
+      <c r="H43" s="59"/>
+      <c r="J43" s="20"/>
+      <c r="L43" s="29"/>
+      <c r="M43" s="29"/>
+      <c r="P43" s="21"/>
+      <c r="R43" s="29"/>
+      <c r="T43" s="45"/>
+      <c r="U43" s="21"/>
+      <c r="Z43" s="47"/>
+    </row>
+    <row r="44" spans="4:26" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D44" s="19"/>
+      <c r="G44" s="47"/>
+      <c r="H44" s="59"/>
+      <c r="J44" s="20"/>
+      <c r="L44" s="29"/>
+      <c r="M44" s="29"/>
+      <c r="P44" s="21"/>
+      <c r="R44" s="29"/>
+      <c r="T44" s="45"/>
+      <c r="U44" s="21"/>
+      <c r="Z44" s="47"/>
+    </row>
+    <row r="45" spans="4:26" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D45" s="19"/>
+      <c r="G45" s="47"/>
+      <c r="H45" s="59"/>
+      <c r="J45" s="20"/>
+      <c r="L45" s="29"/>
+      <c r="M45" s="29"/>
+      <c r="P45" s="21"/>
+      <c r="R45" s="29"/>
+      <c r="T45" s="45"/>
+      <c r="U45" s="21"/>
+      <c r="Z45" s="47"/>
+    </row>
+    <row r="46" spans="4:26" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D46" s="19"/>
+      <c r="G46" s="47"/>
+      <c r="H46" s="59"/>
+      <c r="J46" s="20"/>
+      <c r="L46" s="29"/>
+      <c r="M46" s="29"/>
+      <c r="P46" s="21"/>
+      <c r="R46" s="29"/>
+      <c r="T46" s="45"/>
+      <c r="U46" s="21"/>
+      <c r="Z46" s="47"/>
+    </row>
+    <row r="47" spans="4:26" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D47" s="19"/>
+      <c r="G47" s="47"/>
+      <c r="H47" s="59"/>
+      <c r="J47" s="20"/>
+      <c r="L47" s="29"/>
+      <c r="M47" s="29"/>
+      <c r="P47" s="21"/>
+      <c r="R47" s="29"/>
+      <c r="T47" s="45"/>
+      <c r="U47" s="21"/>
+      <c r="Z47" s="47"/>
+    </row>
+    <row r="48" spans="4:26" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D48" s="19"/>
+      <c r="G48" s="47"/>
+      <c r="H48" s="59"/>
+      <c r="J48" s="20"/>
+      <c r="L48" s="29"/>
+      <c r="M48" s="29"/>
+      <c r="P48" s="21"/>
+      <c r="R48" s="29"/>
+      <c r="T48" s="45"/>
+      <c r="U48" s="21"/>
+      <c r="Z48" s="47"/>
+    </row>
+    <row r="49" spans="4:26" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D49" s="19"/>
+      <c r="G49" s="47"/>
+      <c r="H49" s="59"/>
+      <c r="J49" s="20"/>
+      <c r="L49" s="29"/>
+      <c r="M49" s="29"/>
+      <c r="P49" s="21"/>
+      <c r="R49" s="29"/>
+      <c r="T49" s="45"/>
+      <c r="U49" s="21"/>
+      <c r="Z49" s="47"/>
+    </row>
+    <row r="50" spans="4:26" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D50" s="19"/>
+      <c r="G50" s="47"/>
+      <c r="H50" s="59"/>
+      <c r="J50" s="20"/>
+      <c r="L50" s="29"/>
+      <c r="M50" s="29"/>
+      <c r="P50" s="21"/>
+      <c r="R50" s="29"/>
+      <c r="T50" s="45"/>
+      <c r="U50" s="21"/>
+      <c r="Z50" s="47"/>
+    </row>
+    <row r="51" spans="4:26" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D51" s="19"/>
+      <c r="G51" s="47"/>
+      <c r="H51" s="59"/>
+      <c r="J51" s="20"/>
+      <c r="L51" s="29"/>
+      <c r="M51" s="29"/>
+      <c r="P51" s="21"/>
+      <c r="R51" s="29"/>
+      <c r="T51" s="45"/>
+      <c r="U51" s="21"/>
+      <c r="Z51" s="47"/>
+    </row>
+    <row r="52" spans="4:26" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D52" s="19"/>
+      <c r="G52" s="47"/>
+      <c r="H52" s="59"/>
+      <c r="J52" s="20"/>
+      <c r="L52" s="29"/>
+      <c r="M52" s="29"/>
+      <c r="P52" s="21"/>
+      <c r="R52" s="29"/>
+      <c r="T52" s="45"/>
+      <c r="U52" s="21"/>
+      <c r="Z52" s="47"/>
+    </row>
+    <row r="53" spans="4:26" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D53" s="19"/>
+      <c r="G53" s="47"/>
+      <c r="H53" s="59"/>
+      <c r="J53" s="20"/>
+      <c r="L53" s="29"/>
+      <c r="M53" s="29"/>
+      <c r="P53" s="21"/>
+      <c r="R53" s="29"/>
+      <c r="T53" s="45"/>
+      <c r="U53" s="21"/>
+      <c r="Z53" s="47"/>
+    </row>
+    <row r="54" spans="4:26" x14ac:dyDescent="0.25">
+      <c r="G54" s="48"/>
+      <c r="H54" s="59"/>
+      <c r="J54" s="31"/>
+      <c r="P54" s="21"/>
+      <c r="T54" s="46"/>
+    </row>
+    <row r="55" spans="4:26" x14ac:dyDescent="0.25">
+      <c r="G55" s="48"/>
+      <c r="H55" s="59"/>
+      <c r="J55" s="31"/>
+      <c r="P55" s="21"/>
+      <c r="T55" s="46"/>
+    </row>
+    <row r="56" spans="4:26" x14ac:dyDescent="0.25">
+      <c r="G56" s="48"/>
+      <c r="H56" s="59"/>
+      <c r="J56" s="31"/>
+      <c r="P56" s="21"/>
+      <c r="T56" s="46"/>
+    </row>
+    <row r="57" spans="4:26" x14ac:dyDescent="0.25">
+      <c r="G57" s="48"/>
+      <c r="H57" s="59"/>
+      <c r="J57" s="31"/>
+      <c r="P57" s="21"/>
+      <c r="T57" s="46"/>
+    </row>
+    <row r="58" spans="4:26" x14ac:dyDescent="0.25">
+      <c r="G58" s="48"/>
+      <c r="H58" s="59"/>
+      <c r="J58" s="31"/>
+      <c r="P58" s="21"/>
+      <c r="T58" s="46"/>
+    </row>
+    <row r="59" spans="4:26" x14ac:dyDescent="0.25">
+      <c r="G59" s="48"/>
+      <c r="H59" s="59"/>
+      <c r="J59" s="31"/>
+      <c r="P59" s="21"/>
+      <c r="T59" s="46"/>
+    </row>
+    <row r="60" spans="4:26" x14ac:dyDescent="0.25">
+      <c r="G60" s="48"/>
+      <c r="H60" s="59"/>
+      <c r="J60" s="31"/>
+      <c r="P60" s="21"/>
+      <c r="T60" s="46"/>
+    </row>
+    <row r="61" spans="4:26" x14ac:dyDescent="0.25">
+      <c r="G61" s="48"/>
+      <c r="H61" s="59"/>
+      <c r="J61" s="31"/>
+      <c r="P61" s="21"/>
+      <c r="T61" s="46"/>
+    </row>
+    <row r="62" spans="4:26" x14ac:dyDescent="0.25">
+      <c r="G62" s="48"/>
+      <c r="H62" s="59"/>
+      <c r="J62" s="31"/>
+      <c r="P62" s="21"/>
+      <c r="T62" s="46"/>
+    </row>
+    <row r="63" spans="4:26" x14ac:dyDescent="0.25">
+      <c r="G63" s="48"/>
+      <c r="H63" s="59"/>
+      <c r="J63" s="31"/>
+      <c r="P63" s="21"/>
+      <c r="T63" s="46"/>
+    </row>
+    <row r="64" spans="4:26" x14ac:dyDescent="0.25">
+      <c r="G64" s="48"/>
+      <c r="H64" s="59"/>
+      <c r="J64" s="31"/>
+      <c r="P64" s="21"/>
+      <c r="T64" s="46"/>
+    </row>
+    <row r="65" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G65" s="48"/>
+      <c r="H65" s="59"/>
+      <c r="J65" s="31"/>
+      <c r="P65" s="21"/>
+      <c r="T65" s="46"/>
+    </row>
+    <row r="66" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G66" s="48"/>
+      <c r="H66" s="59"/>
+      <c r="J66" s="31"/>
+      <c r="P66" s="21"/>
+      <c r="T66" s="46"/>
+    </row>
+    <row r="67" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G67" s="48"/>
+      <c r="H67" s="59"/>
+      <c r="J67" s="31"/>
+      <c r="P67" s="21"/>
+      <c r="T67" s="46"/>
+    </row>
+    <row r="68" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G68" s="48"/>
+      <c r="H68" s="59"/>
+      <c r="J68" s="31"/>
+      <c r="P68" s="21"/>
+      <c r="T68" s="46"/>
+    </row>
+    <row r="69" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G69" s="48"/>
+      <c r="H69" s="59"/>
+      <c r="J69" s="31"/>
+      <c r="P69" s="21"/>
+      <c r="T69" s="46"/>
+    </row>
+    <row r="70" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G70" s="48"/>
+      <c r="H70" s="59"/>
+      <c r="J70" s="31"/>
+      <c r="P70" s="21"/>
+      <c r="T70" s="46"/>
+    </row>
+    <row r="71" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G71" s="48"/>
+      <c r="H71" s="59"/>
+      <c r="J71" s="31"/>
+      <c r="P71" s="21"/>
+      <c r="T71" s="46"/>
+    </row>
+    <row r="72" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G72" s="48"/>
+      <c r="H72" s="59"/>
+      <c r="J72" s="31"/>
+      <c r="P72" s="21"/>
+      <c r="T72" s="46"/>
+    </row>
+    <row r="73" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G73" s="48"/>
+      <c r="H73" s="59"/>
+      <c r="J73" s="31"/>
+      <c r="P73" s="21"/>
+      <c r="T73" s="46"/>
+    </row>
+    <row r="74" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G74" s="48"/>
+      <c r="H74" s="59"/>
+      <c r="J74" s="31"/>
+      <c r="P74" s="21"/>
+      <c r="T74" s="46"/>
+    </row>
+    <row r="75" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G75" s="48"/>
+      <c r="H75" s="59"/>
+      <c r="J75" s="31"/>
+      <c r="P75" s="21"/>
+      <c r="T75" s="46"/>
+    </row>
+    <row r="76" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G76" s="48"/>
+      <c r="H76" s="59"/>
+      <c r="J76" s="31"/>
+      <c r="P76" s="21"/>
+      <c r="T76" s="46"/>
+    </row>
+    <row r="77" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G77" s="48"/>
+      <c r="H77" s="59"/>
+      <c r="J77" s="31"/>
+      <c r="P77" s="21"/>
+      <c r="T77" s="46"/>
+    </row>
+    <row r="78" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G78" s="48"/>
+      <c r="H78" s="59"/>
+      <c r="J78" s="31"/>
+      <c r="P78" s="21"/>
+      <c r="T78" s="46"/>
+    </row>
+    <row r="79" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G79" s="48"/>
+      <c r="H79" s="59"/>
+      <c r="J79" s="31"/>
+      <c r="P79" s="21"/>
+      <c r="T79" s="46"/>
+    </row>
+    <row r="80" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G80" s="48"/>
+      <c r="H80" s="59"/>
+      <c r="J80" s="31"/>
+      <c r="P80" s="21"/>
+      <c r="T80" s="46"/>
+    </row>
+    <row r="81" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G81" s="48"/>
+      <c r="H81" s="59"/>
+      <c r="J81" s="31"/>
+      <c r="P81" s="21"/>
+      <c r="T81" s="46"/>
+    </row>
+    <row r="82" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G82" s="48"/>
+      <c r="H82" s="59"/>
+      <c r="J82" s="31"/>
+      <c r="P82" s="21"/>
+      <c r="T82" s="46"/>
+    </row>
+    <row r="83" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G83" s="48"/>
+      <c r="H83" s="59"/>
+      <c r="J83" s="31"/>
+      <c r="P83" s="21"/>
+      <c r="T83" s="46"/>
+    </row>
+    <row r="84" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G84" s="48"/>
+      <c r="H84" s="59"/>
+      <c r="J84" s="31"/>
+      <c r="P84" s="21"/>
+      <c r="T84" s="46"/>
+    </row>
+    <row r="85" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G85" s="48"/>
+      <c r="H85" s="59"/>
+      <c r="J85" s="31"/>
+      <c r="P85" s="21"/>
+      <c r="T85" s="46"/>
+    </row>
+    <row r="86" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G86" s="48"/>
+      <c r="H86" s="59"/>
+      <c r="J86" s="31"/>
+      <c r="P86" s="21"/>
+      <c r="T86" s="46"/>
+    </row>
+    <row r="87" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G87" s="48"/>
+      <c r="H87" s="59"/>
+      <c r="J87" s="31"/>
+      <c r="P87" s="21"/>
+      <c r="T87" s="46"/>
+    </row>
+    <row r="88" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G88" s="48"/>
+      <c r="H88" s="59"/>
+      <c r="J88" s="31"/>
+      <c r="P88" s="21"/>
+      <c r="T88" s="46"/>
+    </row>
+    <row r="89" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G89" s="48"/>
+      <c r="H89" s="59"/>
+      <c r="J89" s="31"/>
+      <c r="P89" s="21"/>
+      <c r="T89" s="46"/>
+    </row>
+    <row r="90" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G90" s="48"/>
+      <c r="H90" s="59"/>
+      <c r="J90" s="31"/>
+      <c r="P90" s="21"/>
+      <c r="T90" s="46"/>
+    </row>
+    <row r="91" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G91" s="48"/>
+      <c r="H91" s="59"/>
+      <c r="J91" s="31"/>
+      <c r="P91" s="21"/>
+      <c r="T91" s="46"/>
+    </row>
+    <row r="92" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G92" s="48"/>
+      <c r="H92" s="59"/>
+      <c r="J92" s="31"/>
+      <c r="P92" s="21"/>
+      <c r="T92" s="46"/>
+    </row>
+    <row r="93" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G93" s="48"/>
+      <c r="H93" s="59"/>
+      <c r="J93" s="31"/>
+      <c r="P93" s="21"/>
+      <c r="T93" s="46"/>
+    </row>
+    <row r="94" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G94" s="48"/>
+      <c r="H94" s="59"/>
+      <c r="J94" s="31"/>
+      <c r="P94" s="21"/>
+      <c r="T94" s="46"/>
+    </row>
+    <row r="95" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G95" s="48"/>
+      <c r="H95" s="59"/>
+      <c r="J95" s="31"/>
+      <c r="P95" s="21"/>
+      <c r="T95" s="46"/>
+    </row>
+    <row r="96" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G96" s="48"/>
+      <c r="H96" s="59"/>
+      <c r="J96" s="31"/>
+      <c r="P96" s="21"/>
+      <c r="T96" s="46"/>
+    </row>
+    <row r="97" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G97" s="48"/>
+      <c r="H97" s="59"/>
+      <c r="J97" s="31"/>
+      <c r="P97" s="21"/>
+      <c r="T97" s="46"/>
+    </row>
+    <row r="98" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G98" s="48"/>
+      <c r="H98" s="59"/>
+      <c r="J98" s="31"/>
+      <c r="P98" s="21"/>
+      <c r="T98" s="46"/>
+    </row>
+    <row r="99" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G99" s="48"/>
+      <c r="H99" s="59"/>
+      <c r="J99" s="31"/>
+      <c r="P99" s="21"/>
+      <c r="T99" s="46"/>
+    </row>
+    <row r="100" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G100" s="48"/>
+      <c r="H100" s="59"/>
+      <c r="J100" s="31"/>
+      <c r="P100" s="21"/>
+      <c r="T100" s="46"/>
+    </row>
+    <row r="101" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G101" s="48"/>
+      <c r="H101" s="59"/>
+      <c r="J101" s="31"/>
+      <c r="P101" s="21"/>
+      <c r="T101" s="46"/>
+    </row>
+    <row r="102" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G102" s="48"/>
+      <c r="H102" s="59"/>
+      <c r="J102" s="31"/>
+      <c r="P102" s="21"/>
+      <c r="T102" s="46"/>
+    </row>
+    <row r="103" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G103" s="48"/>
+      <c r="H103" s="59"/>
+      <c r="J103" s="31"/>
+      <c r="P103" s="21"/>
+      <c r="T103" s="46"/>
+    </row>
+    <row r="104" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G104" s="48"/>
+      <c r="H104" s="59"/>
+      <c r="J104" s="31"/>
+      <c r="P104" s="21"/>
+      <c r="T104" s="46"/>
+    </row>
+    <row r="105" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G105" s="48"/>
+      <c r="H105" s="59"/>
+      <c r="J105" s="31"/>
+      <c r="P105" s="21"/>
+      <c r="T105" s="46"/>
+    </row>
+    <row r="106" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G106" s="48"/>
+      <c r="H106" s="59"/>
+      <c r="J106" s="31"/>
+      <c r="P106" s="21"/>
+      <c r="T106" s="46"/>
+    </row>
+    <row r="107" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G107" s="48"/>
+      <c r="H107" s="59"/>
+      <c r="J107" s="31"/>
+      <c r="P107" s="21"/>
+      <c r="T107" s="46"/>
+    </row>
+    <row r="108" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G108" s="48"/>
+      <c r="H108" s="59"/>
+      <c r="J108" s="31"/>
+      <c r="P108" s="21"/>
+      <c r="T108" s="46"/>
+    </row>
+    <row r="109" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G109" s="48"/>
+      <c r="H109" s="59"/>
+      <c r="J109" s="31"/>
+      <c r="P109" s="21"/>
+      <c r="T109" s="46"/>
+    </row>
+    <row r="110" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G110" s="48"/>
+      <c r="H110" s="59"/>
+      <c r="J110" s="31"/>
+      <c r="P110" s="21"/>
+      <c r="T110" s="46"/>
+    </row>
+    <row r="111" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G111" s="48"/>
+      <c r="H111" s="59"/>
+      <c r="J111" s="31"/>
+      <c r="P111" s="21"/>
+      <c r="T111" s="46"/>
+    </row>
+    <row r="112" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G112" s="48"/>
+      <c r="H112" s="59"/>
+      <c r="J112" s="31"/>
+      <c r="P112" s="21"/>
+      <c r="T112" s="46"/>
+    </row>
+    <row r="113" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G113" s="48"/>
+      <c r="H113" s="59"/>
+      <c r="J113" s="31"/>
+      <c r="P113" s="21"/>
+      <c r="T113" s="46"/>
+    </row>
+    <row r="114" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G114" s="48"/>
+      <c r="H114" s="59"/>
+      <c r="J114" s="31"/>
+      <c r="P114" s="21"/>
+      <c r="T114" s="46"/>
+    </row>
+    <row r="115" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G115" s="48"/>
+      <c r="H115" s="59"/>
+      <c r="J115" s="31"/>
+      <c r="P115" s="21"/>
+      <c r="T115" s="46"/>
+    </row>
+    <row r="116" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G116" s="48"/>
+      <c r="H116" s="59"/>
+      <c r="J116" s="31"/>
+      <c r="P116" s="21"/>
+      <c r="T116" s="46"/>
+    </row>
+    <row r="117" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G117" s="48"/>
+      <c r="H117" s="59"/>
+      <c r="J117" s="31"/>
+      <c r="P117" s="21"/>
+      <c r="T117" s="46"/>
+    </row>
+    <row r="118" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G118" s="48"/>
+      <c r="H118" s="59"/>
+      <c r="J118" s="31"/>
+      <c r="P118" s="21"/>
+      <c r="T118" s="46"/>
+    </row>
+    <row r="119" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G119" s="48"/>
+      <c r="H119" s="59"/>
+      <c r="J119" s="31"/>
+      <c r="P119" s="21"/>
+      <c r="T119" s="46"/>
+    </row>
+    <row r="120" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G120" s="48"/>
+      <c r="H120" s="59"/>
+      <c r="J120" s="31"/>
+      <c r="P120" s="21"/>
+      <c r="T120" s="46"/>
+    </row>
+    <row r="121" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G121" s="48"/>
+      <c r="H121" s="59"/>
+      <c r="J121" s="31"/>
+      <c r="P121" s="21"/>
+      <c r="T121" s="46"/>
+    </row>
+    <row r="122" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G122" s="48"/>
+      <c r="H122" s="59"/>
+      <c r="J122" s="31"/>
+      <c r="P122" s="21"/>
+      <c r="T122" s="46"/>
+    </row>
+    <row r="123" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G123" s="48"/>
+      <c r="H123" s="59"/>
+      <c r="J123" s="31"/>
+      <c r="P123" s="21"/>
+      <c r="T123" s="46"/>
+    </row>
+    <row r="124" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G124" s="48"/>
+      <c r="H124" s="59"/>
+      <c r="J124" s="31"/>
+      <c r="P124" s="21"/>
+      <c r="T124" s="46"/>
+    </row>
+    <row r="125" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G125" s="48"/>
+      <c r="H125" s="59"/>
+      <c r="J125" s="31"/>
+      <c r="P125" s="21"/>
+      <c r="T125" s="46"/>
+    </row>
+    <row r="126" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G126" s="48"/>
+      <c r="H126" s="59"/>
+      <c r="J126" s="31"/>
+      <c r="P126" s="21"/>
+      <c r="T126" s="46"/>
+    </row>
+    <row r="127" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G127" s="48"/>
+      <c r="H127" s="59"/>
+      <c r="J127" s="31"/>
+      <c r="P127" s="21"/>
+      <c r="T127" s="46"/>
+    </row>
+    <row r="128" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G128" s="48"/>
+      <c r="H128" s="59"/>
+      <c r="J128" s="31"/>
+      <c r="P128" s="21"/>
+      <c r="T128" s="46"/>
+    </row>
+    <row r="129" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G129" s="48"/>
+      <c r="H129" s="59"/>
+      <c r="J129" s="31"/>
+      <c r="P129" s="21"/>
+      <c r="T129" s="46"/>
+    </row>
+    <row r="130" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G130" s="48"/>
+      <c r="H130" s="59"/>
+      <c r="J130" s="31"/>
+      <c r="P130" s="21"/>
+      <c r="T130" s="46"/>
+    </row>
+    <row r="131" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G131" s="48"/>
+      <c r="H131" s="59"/>
+      <c r="J131" s="31"/>
+      <c r="P131" s="21"/>
+      <c r="T131" s="46"/>
+    </row>
+    <row r="132" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G132" s="48"/>
+      <c r="H132" s="59"/>
+      <c r="J132" s="31"/>
+      <c r="P132" s="21"/>
+      <c r="T132" s="46"/>
+    </row>
+    <row r="133" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G133" s="48"/>
+      <c r="H133" s="59"/>
+      <c r="J133" s="31"/>
+      <c r="P133" s="21"/>
+      <c r="T133" s="46"/>
+    </row>
+    <row r="134" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G134" s="48"/>
+      <c r="H134" s="59"/>
+      <c r="J134" s="31"/>
+      <c r="P134" s="21"/>
+      <c r="T134" s="46"/>
+    </row>
+    <row r="135" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G135" s="48"/>
+      <c r="H135" s="59"/>
+      <c r="J135" s="31"/>
+      <c r="P135" s="21"/>
+      <c r="T135" s="46"/>
+    </row>
+    <row r="136" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G136" s="48"/>
+      <c r="H136" s="59"/>
+      <c r="J136" s="31"/>
+      <c r="P136" s="21"/>
+      <c r="T136" s="46"/>
+    </row>
+    <row r="137" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G137" s="48"/>
+      <c r="H137" s="59"/>
+      <c r="J137" s="31"/>
+      <c r="P137" s="21"/>
+      <c r="T137" s="46"/>
+    </row>
+    <row r="138" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G138" s="48"/>
+      <c r="H138" s="59"/>
+      <c r="J138" s="31"/>
+      <c r="P138" s="21"/>
+      <c r="T138" s="46"/>
+    </row>
+    <row r="139" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G139" s="48"/>
+      <c r="H139" s="59"/>
+      <c r="J139" s="31"/>
+      <c r="P139" s="21"/>
+      <c r="T139" s="46"/>
+    </row>
+    <row r="140" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G140" s="48"/>
+      <c r="H140" s="59"/>
+      <c r="J140" s="31"/>
+      <c r="P140" s="21"/>
+      <c r="T140" s="46"/>
+    </row>
+    <row r="141" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G141" s="48"/>
+      <c r="H141" s="59"/>
+      <c r="J141" s="31"/>
+      <c r="P141" s="21"/>
+      <c r="T141" s="46"/>
+    </row>
+    <row r="142" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G142" s="48"/>
+      <c r="H142" s="59"/>
+      <c r="J142" s="31"/>
+      <c r="P142" s="21"/>
+      <c r="T142" s="46"/>
+    </row>
+    <row r="143" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G143" s="48"/>
+      <c r="H143" s="59"/>
+      <c r="J143" s="31"/>
+      <c r="P143" s="21"/>
+      <c r="T143" s="46"/>
+    </row>
+    <row r="144" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G144" s="48"/>
+      <c r="H144" s="59"/>
+      <c r="J144" s="31"/>
+      <c r="P144" s="21"/>
+      <c r="T144" s="46"/>
+    </row>
+    <row r="145" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G145" s="48"/>
+      <c r="H145" s="59"/>
+      <c r="J145" s="31"/>
+      <c r="P145" s="21"/>
+      <c r="T145" s="46"/>
+    </row>
+    <row r="146" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G146" s="48"/>
+      <c r="H146" s="59"/>
+      <c r="J146" s="31"/>
+      <c r="P146" s="21"/>
+      <c r="T146" s="46"/>
+    </row>
+    <row r="147" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G147" s="48"/>
+      <c r="H147" s="59"/>
+      <c r="J147" s="31"/>
+      <c r="P147" s="21"/>
+      <c r="T147" s="46"/>
+    </row>
+    <row r="148" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G148" s="48"/>
+      <c r="H148" s="59"/>
+      <c r="J148" s="31"/>
+      <c r="P148" s="21"/>
+      <c r="T148" s="46"/>
+    </row>
+    <row r="149" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G149" s="48"/>
+      <c r="H149" s="59"/>
+      <c r="J149" s="31"/>
+      <c r="P149" s="21"/>
+      <c r="T149" s="46"/>
+    </row>
+    <row r="150" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G150" s="48"/>
+      <c r="H150" s="59"/>
+      <c r="J150" s="31"/>
+      <c r="P150" s="21"/>
+      <c r="T150" s="46"/>
+    </row>
+    <row r="151" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G151" s="48"/>
+      <c r="H151" s="59"/>
+      <c r="J151" s="31"/>
+      <c r="P151" s="21"/>
+      <c r="T151" s="46"/>
+    </row>
+    <row r="152" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G152" s="48"/>
+      <c r="H152" s="59"/>
+      <c r="J152" s="31"/>
+      <c r="P152" s="21"/>
+      <c r="T152" s="46"/>
+    </row>
+    <row r="153" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G153" s="48"/>
+      <c r="H153" s="59"/>
+      <c r="J153" s="31"/>
+      <c r="P153" s="21"/>
+      <c r="T153" s="46"/>
+    </row>
+    <row r="154" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G154" s="48"/>
+      <c r="H154" s="60"/>
+    </row>
+    <row r="155" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G155" s="48"/>
+      <c r="H155" s="60"/>
+    </row>
+    <row r="156" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G156" s="48"/>
+      <c r="H156" s="60"/>
+    </row>
+    <row r="157" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G157" s="48"/>
+      <c r="H157" s="60"/>
+    </row>
+    <row r="158" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G158" s="48"/>
+      <c r="H158" s="60"/>
+    </row>
+    <row r="159" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G159" s="48"/>
+      <c r="H159" s="60"/>
+    </row>
+    <row r="160" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G160" s="48"/>
+      <c r="H160" s="60"/>
+    </row>
+    <row r="161" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G161" s="48"/>
+      <c r="H161" s="60"/>
+    </row>
+    <row r="162" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G162" s="48"/>
+      <c r="H162" s="60"/>
+    </row>
+    <row r="163" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G163" s="48"/>
+      <c r="H163" s="60"/>
+    </row>
+    <row r="164" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G164" s="48"/>
+      <c r="H164" s="60"/>
+    </row>
+    <row r="165" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G165" s="48"/>
+      <c r="H165" s="60"/>
+    </row>
+    <row r="166" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G166" s="48"/>
+      <c r="H166" s="60"/>
+    </row>
+    <row r="167" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G167" s="48"/>
+      <c r="H167" s="60"/>
+    </row>
+    <row r="168" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G168" s="48"/>
+      <c r="H168" s="60"/>
+    </row>
+    <row r="169" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G169" s="48"/>
+      <c r="H169" s="60"/>
+    </row>
+    <row r="170" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G170" s="48"/>
+      <c r="H170" s="60"/>
+    </row>
+    <row r="171" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G171" s="48"/>
+      <c r="H171" s="60"/>
+    </row>
+    <row r="172" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G172" s="48"/>
+      <c r="H172" s="60"/>
+    </row>
+    <row r="173" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G173" s="48"/>
+      <c r="H173" s="60"/>
+    </row>
+    <row r="174" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G174" s="48"/>
+      <c r="H174" s="60"/>
+    </row>
+    <row r="175" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G175" s="48"/>
+      <c r="H175" s="60"/>
+    </row>
+    <row r="176" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G176" s="48"/>
+      <c r="H176" s="60"/>
+    </row>
+    <row r="177" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G177" s="48"/>
+      <c r="H177" s="60"/>
+    </row>
+    <row r="178" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G178" s="48"/>
+      <c r="H178" s="60"/>
+    </row>
+    <row r="179" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G179" s="48"/>
+      <c r="H179" s="60"/>
+    </row>
+    <row r="180" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G180" s="48"/>
+      <c r="H180" s="60"/>
+    </row>
+    <row r="181" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G181" s="48"/>
+      <c r="H181" s="60"/>
+    </row>
+    <row r="182" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G182" s="48"/>
+      <c r="H182" s="60"/>
+    </row>
+    <row r="183" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G183" s="48"/>
+      <c r="H183" s="60"/>
+    </row>
+    <row r="184" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G184" s="48"/>
+      <c r="H184" s="60"/>
+    </row>
+    <row r="185" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G185" s="48"/>
+      <c r="H185" s="60"/>
+    </row>
+    <row r="186" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G186" s="48"/>
+      <c r="H186" s="60"/>
+    </row>
+    <row r="187" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G187" s="48"/>
+      <c r="H187" s="60"/>
+    </row>
+    <row r="188" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G188" s="48"/>
+      <c r="H188" s="60"/>
+    </row>
+    <row r="189" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G189" s="48"/>
+      <c r="H189" s="60"/>
+    </row>
+    <row r="190" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G190" s="48"/>
+      <c r="H190" s="60"/>
+    </row>
+    <row r="191" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G191" s="48"/>
+      <c r="H191" s="60"/>
+    </row>
+    <row r="192" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G192" s="48"/>
+      <c r="H192" s="60"/>
+    </row>
+    <row r="193" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G193" s="48"/>
+      <c r="H193" s="60"/>
+    </row>
+    <row r="194" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G194" s="48"/>
+      <c r="H194" s="60"/>
+    </row>
+    <row r="195" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G195" s="48"/>
+      <c r="H195" s="60"/>
+    </row>
+    <row r="196" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G196" s="48"/>
+      <c r="H196" s="60"/>
+    </row>
+    <row r="197" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G197" s="48"/>
+      <c r="H197" s="60"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="K1:S1"/>
+    <mergeCell ref="U1:AA1"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="S2:S3"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="N2:P2"/>
+  </mergeCells>
+  <phoneticPr fontId="37" type="noConversion"/>
+  <conditionalFormatting sqref="A4:I10000">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>$R4 = "Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K4:S10000">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>$R4 = "Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U4:AA10000">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$R4 = "Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;G</oddHeader>
+  </headerFooter>
+  <legacyDrawingHF r:id="rId2"/>
+  <picture r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -3785,7 +5515,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -3793,7 +5523,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -3801,7 +5531,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>33</v>
       </c>
@@ -3809,7 +5539,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -3817,7 +5547,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -3825,7 +5555,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>39</v>
       </c>
@@ -3833,7 +5563,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>41</v>
       </c>
@@ -3841,7 +5571,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>43</v>
       </c>
@@ -3849,7 +5579,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>45</v>
       </c>
@@ -3857,7 +5587,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:2" s="26" customFormat="1">
+    <row r="13" spans="1:2" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="26" t="s">
         <v>70</v>
       </c>
@@ -3865,7 +5595,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>47</v>
       </c>
@@ -3874,6 +5604,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="37" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter>

</xml_diff>